<commit_message>
updated BOM, fixed footprints
</commit_message>
<xml_diff>
--- a/SPEX HAB2 BOM.xlsx
+++ b/SPEX HAB2 BOM.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Turnkey" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$56</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$58</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="370">
   <si>
     <t>Description</t>
   </si>
@@ -1070,6 +1070,102 @@
   </si>
   <si>
     <t>International Rectifier</t>
+  </si>
+  <si>
+    <t>MF-LSMF260X-2</t>
+  </si>
+  <si>
+    <t>652-MF-LSMF260X-2</t>
+  </si>
+  <si>
+    <t>Resetable fuse</t>
+  </si>
+  <si>
+    <t>3121</t>
+  </si>
+  <si>
+    <t>MMBT3906LT1G</t>
+  </si>
+  <si>
+    <t>863-MMBT3906LT1G</t>
+  </si>
+  <si>
+    <t>http://www.mouser.com/ds/2/308/MMBT3906LT1-D-112192.pdf</t>
+  </si>
+  <si>
+    <t>BJT Transistor</t>
+  </si>
+  <si>
+    <t>SOT-23</t>
+  </si>
+  <si>
+    <t>DMG2302U-7</t>
+  </si>
+  <si>
+    <t>621-DMG2302U-7</t>
+  </si>
+  <si>
+    <t>Enable pin Nchannel Mosfet</t>
+  </si>
+  <si>
+    <t>SOT23-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diodes Incorportated </t>
+  </si>
+  <si>
+    <t>L102</t>
+  </si>
+  <si>
+    <t>L103</t>
+  </si>
+  <si>
+    <t>2.2uH Inductor</t>
+  </si>
+  <si>
+    <t>3.3uH Inductor</t>
+  </si>
+  <si>
+    <t>BZT52C16-7-F</t>
+  </si>
+  <si>
+    <t>621-BZT52C16-F</t>
+  </si>
+  <si>
+    <t>863-BAV99WT1G</t>
+  </si>
+  <si>
+    <t>BAV99WT1G</t>
+  </si>
+  <si>
+    <t>TYS50402R2N-10</t>
+  </si>
+  <si>
+    <t>875-TYS50402R2N-10</t>
+  </si>
+  <si>
+    <t>Laird Technologies</t>
+  </si>
+  <si>
+    <t>NRS8030T3R3MJGJ</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>963-NRS8030T3R3MJGJ</t>
+  </si>
+  <si>
+    <t>8030</t>
+  </si>
+  <si>
+    <t>B340-13-F</t>
+  </si>
+  <si>
+    <t>621-B340-F</t>
+  </si>
+  <si>
+    <t>input diode</t>
   </si>
 </sst>
 </file>
@@ -1730,10 +1826,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R114"/>
+  <dimension ref="A1:R116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2542,7 +2638,7 @@
         <v>0.52</v>
       </c>
       <c r="H31" s="19">
-        <f t="shared" ref="H31:H52" si="2">(B31*G31)</f>
+        <f t="shared" ref="H31:H54" si="2">(B31*G31)</f>
         <v>1.56</v>
       </c>
       <c r="I31" s="17" t="s">
@@ -2563,16 +2659,28 @@
       <c r="C32" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="17"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="19"/>
+      <c r="D32" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="G32" s="19">
+        <v>0.37</v>
+      </c>
       <c r="H32" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="20"/>
+        <v>0.74</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>349</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>350</v>
+      </c>
       <c r="K32" s="17" t="s">
         <v>190</v>
       </c>
@@ -2621,18 +2729,33 @@
       <c r="C34" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="19"/>
+      <c r="D34" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="G34" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H34" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I34" s="17"/>
-      <c r="J34" s="20"/>
+        <v>0.1</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="J34" s="20" t="s">
+        <v>346</v>
+      </c>
       <c r="K34" s="17" t="s">
         <v>190</v>
+      </c>
+      <c r="L34" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
@@ -2798,13 +2921,21 @@
       <c r="C39" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="19"/>
+      <c r="D39" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="G39" s="19">
+        <v>0.19</v>
+      </c>
       <c r="H39" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="I39" s="17"/>
       <c r="J39" s="20"/>
@@ -2825,10 +2956,18 @@
       <c r="C40" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="19"/>
+      <c r="D40" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>358</v>
+      </c>
+      <c r="G40" s="19">
+        <v>0</v>
+      </c>
       <c r="H40" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2850,17 +2989,27 @@
         <v>1</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="17"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="19"/>
+        <v>352</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="E41" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="G41" s="19">
+        <v>0.38</v>
+      </c>
       <c r="H41" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I41" s="17"/>
+        <f>(B41*G41)</f>
+        <v>0.38</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>354</v>
+      </c>
       <c r="J41" s="20"/>
       <c r="K41" s="17" t="s">
         <v>190</v>
@@ -2877,18 +3026,30 @@
         <v>1</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="17"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="19"/>
+        <v>353</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="E42" s="15" t="s">
+        <v>363</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="G42" s="19">
+        <v>0.48</v>
+      </c>
       <c r="H42" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="20"/>
+        <v>0.48</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="J42" s="20" t="s">
+        <v>366</v>
+      </c>
       <c r="K42" s="17" t="s">
         <v>190</v>
       </c>
@@ -2897,44 +3058,41 @@
       <c r="N42" s="1"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="33">
+      <c r="A43" s="34">
         <v>33</v>
       </c>
       <c r="B43" s="15">
-        <v>2</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>214</v>
+        <v>351</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>213</v>
+        <v>367</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>195</v>
+        <v>368</v>
       </c>
       <c r="G43" s="19">
-        <v>1.43</v>
+        <v>0.34</v>
       </c>
       <c r="H43" s="19">
         <f t="shared" si="2"/>
-        <v>2.86</v>
+        <v>0.34</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="J43" s="21"/>
+        <v>369</v>
+      </c>
+      <c r="J43" s="20"/>
       <c r="K43" s="17" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
-      <c r="R43" s="2" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="33">
@@ -2943,123 +3101,124 @@
       <c r="B44" s="15">
         <v>1</v>
       </c>
-      <c r="C44" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="19"/>
+      <c r="C44" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="F44" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="G44" s="19">
+        <v>0.46</v>
+      </c>
       <c r="H44" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="17"/>
+        <v>0.46</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="J44" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="L44" s="3"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A45" s="33">
         <v>35</v>
       </c>
       <c r="B45" s="15">
-        <v>1</v>
-      </c>
-      <c r="C45" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D45" s="17"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="19"/>
+        <v>2</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="G45" s="19">
+        <v>1.43</v>
+      </c>
       <c r="H45" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="17"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="17"/>
+        <v>2.86</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="J45" s="21"/>
+      <c r="K45" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="L45" s="3"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
+      <c r="R45" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="33">
+      <c r="A46" s="34">
         <v>36</v>
       </c>
       <c r="B46" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>200</v>
-      </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="15" t="s">
-        <v>202</v>
-      </c>
-      <c r="G46" s="19">
-        <v>1.5</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D46" s="17"/>
+      <c r="E46" s="15"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="19"/>
       <c r="H46" s="19">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="J46" s="36" t="s">
-        <v>293</v>
-      </c>
-      <c r="K46" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>201</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I46" s="17"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="3"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="33">
         <v>37</v>
       </c>
       <c r="B47" s="15">
-        <v>7</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="G47" s="19">
-        <v>0.72</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="15"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="19"/>
       <c r="H47" s="19">
         <f t="shared" si="2"/>
-        <v>5.04</v>
-      </c>
-      <c r="I47" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="J47" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="K47" s="17" t="s">
-        <v>197</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I47" s="17"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="17"/>
       <c r="L47" s="3"/>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
@@ -3071,112 +3230,105 @@
       <c r="B48" s="15">
         <v>4</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D48" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E48" s="15" t="s">
-        <v>219</v>
-      </c>
+      <c r="C48" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E48" s="17"/>
       <c r="F48" s="15" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="G48" s="19">
-        <v>0.1</v>
+        <v>1.5</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="I48" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="J48" s="20" t="s">
-        <v>188</v>
+        <v>6</v>
+      </c>
+      <c r="I48" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="J48" s="36" t="s">
+        <v>293</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="L48" s="3" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="R48" s="2" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="14">
+      <c r="A49" s="34">
         <v>39</v>
       </c>
       <c r="B49" s="15">
-        <v>18</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>220</v>
+        <v>7</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="F49" s="16" t="s">
-        <v>224</v>
+        <v>198</v>
+      </c>
+      <c r="F49" s="15" t="s">
+        <v>199</v>
       </c>
       <c r="G49" s="19">
-        <v>0.1</v>
+        <v>0.72</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>5.04</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="J49" s="20" t="s">
-        <v>188</v>
+        <v>208</v>
+      </c>
+      <c r="J49" s="17" t="s">
+        <v>293</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>190</v>
-      </c>
+        <v>197</v>
+      </c>
+      <c r="L49" s="3"/>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="R49" s="2" t="s">
-        <v>221</v>
-      </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A50" s="14">
+      <c r="A50" s="33">
         <v>40</v>
       </c>
       <c r="B50" s="15">
-        <v>2</v>
-      </c>
-      <c r="C50" s="27" t="s">
-        <v>56</v>
+        <v>4</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>54</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G50" s="19">
         <v>0.1</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J50" s="20" t="s">
         <v>188</v>
@@ -3184,37 +3336,43 @@
       <c r="K50" s="17" t="s">
         <v>190</v>
       </c>
+      <c r="L50" s="3" t="s">
+        <v>222</v>
+      </c>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
+      <c r="R50" s="2" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="14">
+      <c r="A51" s="33">
         <v>41</v>
       </c>
       <c r="B51" s="15">
-        <v>3</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>60</v>
+        <v>18</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="F51" s="15" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>224</v>
       </c>
       <c r="G51" s="19">
         <v>0.1</v>
       </c>
       <c r="H51" s="19">
         <f t="shared" si="2"/>
-        <v>0.30000000000000004</v>
+        <v>1.8</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>231</v>
+        <v>59</v>
       </c>
       <c r="J51" s="20" t="s">
         <v>188</v>
@@ -3222,40 +3380,40 @@
       <c r="K51" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L51" t="s">
-        <v>232</v>
-      </c>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
+      <c r="R51" s="2" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="14">
+      <c r="A52" s="34">
         <v>42</v>
       </c>
       <c r="B52" s="15">
-        <v>1</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>61</v>
+        <v>2</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>56</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="G52" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H52" s="19">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="I52" s="17" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="J52" s="20" t="s">
         <v>188</v>
@@ -3263,40 +3421,37 @@
       <c r="K52" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L52" t="s">
-        <v>237</v>
-      </c>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="14">
+      <c r="A53" s="33">
         <v>43</v>
       </c>
       <c r="B53" s="15">
-        <v>5</v>
-      </c>
-      <c r="C53" s="17" t="s">
-        <v>63</v>
+        <v>3</v>
+      </c>
+      <c r="C53" s="27" t="s">
+        <v>60</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G53" s="19">
         <v>0.1</v>
       </c>
       <c r="H53" s="19">
-        <f t="shared" ref="H53:H92" si="3">(B53*G53)</f>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I53" s="17" t="s">
-        <v>64</v>
+        <v>231</v>
       </c>
       <c r="J53" s="20" t="s">
         <v>188</v>
@@ -3304,119 +3459,123 @@
       <c r="K53" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L53" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="R53" s="2" t="s">
-        <v>221</v>
-      </c>
+      <c r="L53" t="s">
+        <v>232</v>
+      </c>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="14">
+      <c r="A54" s="33">
         <v>44</v>
       </c>
       <c r="B54" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D54" s="17" t="s">
         <v>235</v>
       </c>
-      <c r="E54" s="17" t="s">
-        <v>241</v>
+      <c r="E54" s="15" t="s">
+        <v>236</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G54" s="19">
         <v>0.08</v>
       </c>
       <c r="H54" s="19">
+        <f t="shared" si="2"/>
+        <v>0.08</v>
+      </c>
+      <c r="I54" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="J54" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K54" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L54" t="s">
+        <v>237</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="34">
+        <v>45</v>
+      </c>
+      <c r="B55" s="15">
+        <v>5</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="F55" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="G55" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H55" s="19">
+        <f t="shared" ref="H55:H94" si="3">(B55*G55)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I55" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="J55" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K55" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="R55" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="33">
+        <v>46</v>
+      </c>
+      <c r="B56" s="15">
+        <v>2</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="F56" s="15" t="s">
+        <v>242</v>
+      </c>
+      <c r="G56" s="19">
+        <v>0.08</v>
+      </c>
+      <c r="H56" s="19">
         <f t="shared" si="3"/>
         <v>0.16</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I56" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="J54" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="K54" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="14">
-        <v>45</v>
-      </c>
-      <c r="B55" s="15">
-        <v>2</v>
-      </c>
-      <c r="C55" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D55" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E55" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>244</v>
-      </c>
-      <c r="G55" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="H55" s="19">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="I55" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J55" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="K55" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L55" s="31" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="14">
-        <v>46</v>
-      </c>
-      <c r="B56" s="15">
-        <v>1</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E56" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="F56" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="G56" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="H56" s="19">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="J56" s="20" t="s">
         <v>188</v>
@@ -3425,27 +3584,27 @@
         <v>190</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="14">
+      <c r="A57" s="33">
         <v>47</v>
       </c>
       <c r="B57" s="15">
         <v>2</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D57" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="E57" s="15" t="s">
-        <v>249</v>
+      <c r="E57" s="17" t="s">
+        <v>243</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G57" s="19">
         <v>0.1</v>
@@ -3455,7 +3614,7 @@
         <v>0.2</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="J57" s="20" t="s">
         <v>188</v>
@@ -3463,28 +3622,28 @@
       <c r="K57" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L57" s="3" t="s">
-        <v>222</v>
+      <c r="L57" s="31" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="14">
+      <c r="A58" s="34">
         <v>48</v>
       </c>
       <c r="B58" s="15">
         <v>1</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="25" t="s">
-        <v>252</v>
-      </c>
-      <c r="E58" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="F58" s="17" t="s">
-        <v>251</v>
+        <v>69</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="F58" s="15" t="s">
+        <v>247</v>
       </c>
       <c r="G58" s="19">
         <v>0.1</v>
@@ -3494,7 +3653,7 @@
         <v>0.1</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J58" s="20" t="s">
         <v>188</v>
@@ -3502,38 +3661,38 @@
       <c r="K58" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L58" t="s">
-        <v>253</v>
+      <c r="L58" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A59" s="14">
+      <c r="A59" s="33">
         <v>49</v>
       </c>
       <c r="B59" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>220</v>
       </c>
       <c r="E59" s="15" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G59" s="19">
         <v>0.1</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J59" s="20" t="s">
         <v>188</v>
@@ -3546,33 +3705,33 @@
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="14">
+      <c r="A60" s="33">
         <v>50</v>
       </c>
       <c r="B60" s="15">
         <v>1</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>257</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>258</v>
+        <v>73</v>
+      </c>
+      <c r="D60" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="E60" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>251</v>
       </c>
       <c r="G60" s="19">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="3"/>
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J60" s="20" t="s">
         <v>188</v>
@@ -3580,38 +3739,38 @@
       <c r="K60" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L60" s="3" t="s">
-        <v>259</v>
+      <c r="L60" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="14">
+      <c r="A61" s="34">
         <v>51</v>
       </c>
       <c r="B61" s="15">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>263</v>
-      </c>
-      <c r="F61" s="21" t="s">
-        <v>264</v>
+        <v>75</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>255</v>
       </c>
       <c r="G61" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="3"/>
-        <v>0.64</v>
+        <v>0.1</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J61" s="20" t="s">
         <v>188</v>
@@ -3619,36 +3778,38 @@
       <c r="K61" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L61" s="3"/>
+      <c r="L61" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A62" s="14">
+      <c r="A62" s="33">
         <v>52</v>
       </c>
       <c r="B62" s="15">
         <v>1</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D62" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="F62" s="21" t="s">
-        <v>272</v>
+        <v>77</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F62" s="15" t="s">
+        <v>258</v>
       </c>
       <c r="G62" s="19">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="J62" s="20" t="s">
         <v>188</v>
@@ -3657,37 +3818,37 @@
         <v>190</v>
       </c>
       <c r="L62" s="3" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="14">
+      <c r="A63" s="33">
         <v>53</v>
       </c>
       <c r="B63" s="15">
         <v>8</v>
       </c>
       <c r="C63" s="17" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>260</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G63" s="19">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="3"/>
-        <v>0.32</v>
+        <v>0.64</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>270</v>
+        <v>81</v>
       </c>
       <c r="J63" s="20" t="s">
         <v>188</v>
@@ -3698,72 +3859,72 @@
       <c r="L63" s="3"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="14">
+      <c r="A64" s="34">
         <v>54</v>
       </c>
       <c r="B64" s="15">
         <v>1</v>
       </c>
-      <c r="C64" s="32" t="s">
-        <v>265</v>
+      <c r="C64" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="E64" s="21" t="s">
-        <v>266</v>
+        <v>273</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>271</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="G64" s="19">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="3"/>
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J64" s="20" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="K64" s="17" t="s">
         <v>190</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A65" s="14">
+      <c r="A65" s="33">
         <v>55</v>
       </c>
       <c r="B65" s="15">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>84</v>
+        <v>269</v>
       </c>
       <c r="D65" s="20" t="s">
         <v>260</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="G65" s="19">
         <v>0.04</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.32</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J65" s="20" t="s">
         <v>188</v>
@@ -3771,75 +3932,75 @@
       <c r="K65" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L65" s="3" t="s">
-        <v>278</v>
-      </c>
+      <c r="L65" s="3"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="14">
+      <c r="A66" s="33">
         <v>56</v>
       </c>
       <c r="B66" s="15">
         <v>1</v>
       </c>
-      <c r="C66" s="17" t="s">
-        <v>85</v>
+      <c r="C66" s="32" t="s">
+        <v>265</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="G66" s="19">
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="3"/>
-        <v>0.11</v>
+        <v>0.02</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="K66" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L66" s="3"/>
+      <c r="L66" s="3" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="14">
+      <c r="A67" s="34">
         <v>57</v>
       </c>
       <c r="B67" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G67" s="19">
-        <v>0.19</v>
+        <v>0.04</v>
       </c>
       <c r="H67" s="19">
         <f t="shared" si="3"/>
-        <v>0.38</v>
+        <v>0.04</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>87</v>
+        <v>275</v>
       </c>
       <c r="J67" s="20" t="s">
         <v>188</v>
@@ -3848,40 +4009,40 @@
         <v>190</v>
       </c>
       <c r="L67" s="3" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A68" s="14">
+      <c r="A68" s="33">
         <v>58</v>
       </c>
       <c r="B68" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D68" s="20" t="s">
         <v>273</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="G68" s="19">
-        <v>0.5</v>
+        <v>0.11</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.11</v>
       </c>
       <c r="I68" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J68" s="20" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="K68" s="17" t="s">
         <v>190</v>
@@ -3889,36 +4050,36 @@
       <c r="L68" s="3"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="14">
+      <c r="A69" s="33">
         <v>59</v>
       </c>
       <c r="B69" s="15">
         <v>2</v>
       </c>
       <c r="C69" s="17" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D69" s="20" t="s">
         <v>284</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="G69" s="19">
-        <v>0.5</v>
+        <v>0.19</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.38</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="K69" s="17" t="s">
         <v>190</v>
@@ -3928,33 +4089,33 @@
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="14">
+      <c r="A70" s="34">
         <v>60</v>
       </c>
       <c r="B70" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>291</v>
+        <v>273</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G70" s="19">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>1</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J70" s="20" t="s">
         <v>215</v>
@@ -3962,179 +4123,201 @@
       <c r="K70" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L70" s="3" t="s">
-        <v>292</v>
-      </c>
+      <c r="L70" s="3"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="14">
+      <c r="A71" s="33">
         <v>61</v>
       </c>
       <c r="B71" s="15">
-        <v>7</v>
-      </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>204</v>
+        <v>2</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="E71" s="21" t="s">
+        <v>287</v>
+      </c>
+      <c r="F71" s="21" t="s">
+        <v>288</v>
       </c>
       <c r="G71" s="19">
-        <v>0.31</v>
+        <v>0.5</v>
       </c>
       <c r="H71" s="19">
         <f t="shared" si="3"/>
-        <v>2.17</v>
+        <v>1</v>
       </c>
       <c r="I71" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="J71" s="20"/>
-      <c r="K71" s="17"/>
+        <v>91</v>
+      </c>
+      <c r="J71" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="K71" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="L71" s="3" t="s">
-        <v>206</v>
+        <v>283</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="14">
+      <c r="A72" s="33">
         <v>62</v>
       </c>
       <c r="B72" s="15">
-        <v>14</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" s="15">
-        <v>1722533123</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>211</v>
+        <v>3</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="E72" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="F72" s="21" t="s">
+        <v>290</v>
       </c>
       <c r="G72" s="19">
-        <v>0.152</v>
+        <v>0.1</v>
       </c>
       <c r="H72" s="19">
         <f t="shared" si="3"/>
-        <v>2.1280000000000001</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I72" s="17" t="s">
-        <v>209</v>
-      </c>
-      <c r="J72" s="20"/>
-      <c r="K72" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="J72" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="K72" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="L72" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="R72" s="2" t="s">
-        <v>194</v>
+        <v>292</v>
       </c>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="37"/>
-      <c r="C73" s="38"/>
-      <c r="D73" s="38"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="37"/>
-      <c r="G73" s="39"/>
-      <c r="H73" s="39"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="40"/>
-      <c r="K73" s="37"/>
-      <c r="L73" s="3"/>
+      <c r="A73" s="34">
+        <v>63</v>
+      </c>
+      <c r="B73" s="15">
+        <v>7</v>
+      </c>
+      <c r="C73" s="17"/>
+      <c r="D73" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E73" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F73" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G73" s="19">
+        <v>0.31</v>
+      </c>
+      <c r="H73" s="19">
+        <f t="shared" si="3"/>
+        <v>2.17</v>
+      </c>
+      <c r="I73" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="J73" s="20"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="3" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="35">
-        <v>1</v>
+      <c r="A74" s="33">
+        <v>64</v>
       </c>
       <c r="B74" s="15">
-        <v>1</v>
-      </c>
-      <c r="C74" s="17" t="s">
-        <v>15</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C74" s="17"/>
       <c r="D74" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="E74" s="17" t="s">
-        <v>28</v>
+        <v>98</v>
+      </c>
+      <c r="E74" s="15">
+        <v>1722533123</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>152</v>
+        <v>211</v>
       </c>
       <c r="G74" s="19">
-        <v>1.4</v>
+        <v>0.152</v>
       </c>
       <c r="H74" s="19">
         <f t="shared" si="3"/>
-        <v>1.4</v>
+        <v>2.1280000000000001</v>
       </c>
       <c r="I74" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="J74" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="K74" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L74" s="3"/>
+        <v>209</v>
+      </c>
+      <c r="J74" s="20"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="R74" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A75" s="35">
-        <v>2</v>
-      </c>
-      <c r="B75" s="15">
-        <v>1</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D75" s="17"/>
-      <c r="E75" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="F75" s="15"/>
-      <c r="G75" s="19"/>
-      <c r="H75" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I75" s="17"/>
-      <c r="J75" s="20"/>
-      <c r="K75" s="17" t="s">
-        <v>190</v>
-      </c>
+      <c r="A75" s="37"/>
+      <c r="B75" s="37"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="37"/>
+      <c r="G75" s="39"/>
+      <c r="H75" s="39"/>
+      <c r="I75" s="38"/>
+      <c r="J75" s="40"/>
+      <c r="K75" s="37"/>
       <c r="L75" s="3"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="35">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B76" s="15">
         <v>1</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D76" s="17"/>
+        <v>15</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>139</v>
+      </c>
       <c r="E76" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F76" s="15"/>
-      <c r="G76" s="19"/>
+        <v>28</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="G76" s="19">
+        <v>1.4</v>
+      </c>
       <c r="H76" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I76" s="17"/>
-      <c r="J76" s="20"/>
+        <v>1.4</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="J76" s="20" t="s">
+        <v>294</v>
+      </c>
       <c r="K76" s="17" t="s">
         <v>190</v>
       </c>
@@ -4142,17 +4325,17 @@
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B77" s="15">
         <v>1</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F77" s="15"/>
       <c r="G77" s="19"/>
@@ -4169,76 +4352,53 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B78" s="15">
         <v>1</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="17" t="s">
-        <v>336</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D78" s="17"/>
       <c r="E78" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="F78" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="G78" s="19">
-        <v>1.56</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="F78" s="15"/>
+      <c r="G78" s="19"/>
       <c r="H78" s="19">
         <f t="shared" si="3"/>
-        <v>1.56</v>
-      </c>
-      <c r="I78" s="17" t="s">
-        <v>297</v>
-      </c>
-      <c r="J78" s="20" t="s">
-        <v>298</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I78" s="17"/>
+      <c r="J78" s="20"/>
       <c r="K78" s="17" t="s">
         <v>190</v>
       </c>
       <c r="L78" s="3"/>
-      <c r="R78" s="2" t="s">
-        <v>194</v>
-      </c>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="35">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B79" s="15">
         <v>1</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="D79" s="17" t="s">
-        <v>337</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D79" s="17"/>
       <c r="E79" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F79" s="15" t="s">
-        <v>299</v>
-      </c>
-      <c r="G79" s="19">
-        <v>0.86</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="F79" s="15"/>
+      <c r="G79" s="19"/>
       <c r="H79" s="19">
         <f t="shared" si="3"/>
-        <v>0.86</v>
-      </c>
-      <c r="I79" s="17" t="s">
-        <v>300</v>
-      </c>
-      <c r="J79" s="20" t="s">
-        <v>301</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I79" s="17"/>
+      <c r="J79" s="20"/>
       <c r="K79" s="17" t="s">
         <v>190</v>
       </c>
@@ -4246,73 +4406,90 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="35">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B80" s="15">
         <v>1</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D80" s="17"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="19"/>
+        <v>17</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="F80" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="G80" s="19">
+        <v>1.56</v>
+      </c>
       <c r="H80" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I80" s="17"/>
-      <c r="J80" s="20"/>
-      <c r="K80" s="15"/>
+        <v>1.56</v>
+      </c>
+      <c r="I80" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>298</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>190</v>
+      </c>
       <c r="L80" s="3"/>
+      <c r="R80" s="2" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="35">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B81" s="15">
         <v>1</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>98</v>
+        <v>337</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F81" s="15" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="G81" s="19">
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="H81" s="19">
         <f t="shared" si="3"/>
-        <v>0.67</v>
+        <v>0.86</v>
       </c>
       <c r="I81" s="17" t="s">
-        <v>107</v>
+        <v>300</v>
       </c>
       <c r="J81" s="20" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="K81" s="17" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="L81" s="3"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="35">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B82" s="15">
         <v>1</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="D82" s="17"/>
       <c r="E82" s="15"/>
@@ -4329,117 +4506,103 @@
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="35">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B83" s="15">
         <v>1</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D83" s="17"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="19"/>
+        <v>50</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E83" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="G83" s="19">
+        <v>0.67</v>
+      </c>
       <c r="H83" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J83" s="20"/>
-      <c r="K83" s="15"/>
+        <v>0.67</v>
+      </c>
+      <c r="I83" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="J83" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="K83" s="17" t="s">
+        <v>197</v>
+      </c>
       <c r="L83" s="3"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84" s="35">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B84" s="15">
         <v>1</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D84" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>312</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>313</v>
-      </c>
-      <c r="G84" s="19">
-        <v>0.1</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D84" s="17"/>
+      <c r="E84" s="15"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="19"/>
       <c r="H84" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I84" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="J84" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="K84" s="17" t="s">
-        <v>190</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I84" s="17"/>
+      <c r="J84" s="20"/>
+      <c r="K84" s="15"/>
       <c r="L84" s="3"/>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85" s="35">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B85" s="15">
         <v>1</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>306</v>
-      </c>
-      <c r="F85" s="15" t="s">
-        <v>307</v>
-      </c>
-      <c r="G85" s="19">
-        <v>0.1</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="D85" s="17"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="19"/>
       <c r="H85" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I85" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J85" s="20" t="s">
-        <v>216</v>
-      </c>
-      <c r="K85" s="17" t="s">
-        <v>190</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J85" s="20"/>
+      <c r="K85" s="15"/>
       <c r="L85" s="3"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="35">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B86" s="15">
         <v>1</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="G86" s="19">
         <v>0.1</v>
@@ -4449,7 +4612,7 @@
         <v>0.1</v>
       </c>
       <c r="I86" s="17" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="J86" s="20" t="s">
         <v>216</v>
@@ -4457,38 +4620,36 @@
       <c r="K86" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L86" s="3" t="s">
-        <v>237</v>
-      </c>
+      <c r="L86" s="3"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="35">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B87" s="15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="G87" s="19">
         <v>0.1</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I87" s="17" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="J87" s="20" t="s">
         <v>216</v>
@@ -4496,28 +4657,26 @@
       <c r="K87" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L87" s="3" t="s">
-        <v>222</v>
-      </c>
+      <c r="L87" s="3"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="35">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B88" s="15">
         <v>1</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D88" s="17" t="s">
         <v>235</v>
       </c>
       <c r="E88" s="15" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F88" s="15" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="G88" s="19">
         <v>0.1</v>
@@ -4527,7 +4686,7 @@
         <v>0.1</v>
       </c>
       <c r="I88" s="17" t="s">
-        <v>66</v>
+        <v>114</v>
       </c>
       <c r="J88" s="20" t="s">
         <v>216</v>
@@ -4536,72 +4695,96 @@
         <v>190</v>
       </c>
       <c r="L88" s="3" t="s">
-        <v>316</v>
+        <v>237</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="35">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B89" s="15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="D89" s="17"/>
-      <c r="E89" s="21"/>
-      <c r="F89" s="21"/>
-      <c r="G89" s="19"/>
+        <v>115</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>310</v>
+      </c>
+      <c r="F89" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="G89" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H89" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I89" s="17"/>
+        <v>0.2</v>
+      </c>
+      <c r="I89" s="17" t="s">
+        <v>64</v>
+      </c>
       <c r="J89" s="20" t="s">
         <v>216</v>
       </c>
       <c r="K89" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L89" s="3"/>
+      <c r="L89" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90" s="35">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B90" s="15">
         <v>1</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="D90" s="17"/>
-      <c r="E90" s="21"/>
-      <c r="F90" s="21"/>
-      <c r="G90" s="19"/>
+        <v>116</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="G90" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H90" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I90" s="17"/>
+        <v>0.1</v>
+      </c>
+      <c r="I90" s="17" t="s">
+        <v>66</v>
+      </c>
       <c r="J90" s="20" t="s">
         <v>216</v>
       </c>
       <c r="K90" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L90" s="3"/>
+      <c r="L90" s="3" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91" s="35">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B91" s="15">
         <v>1</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D91" s="17"/>
       <c r="E91" s="21"/>
@@ -4613,7 +4796,7 @@
       </c>
       <c r="I91" s="17"/>
       <c r="J91" s="20" t="s">
-        <v>305</v>
+        <v>216</v>
       </c>
       <c r="K91" s="17" t="s">
         <v>190</v>
@@ -4622,13 +4805,13 @@
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="35">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B92" s="15">
         <v>1</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D92" s="17"/>
       <c r="E92" s="21"/>
@@ -4649,211 +4832,265 @@
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93" s="35">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B93" s="15">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="D93" s="17" t="s">
-        <v>260</v>
-      </c>
-      <c r="E93" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="F93" s="21" t="s">
-        <v>318</v>
-      </c>
-      <c r="G93" s="19">
-        <v>0.05</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="D93" s="17"/>
+      <c r="E93" s="21"/>
+      <c r="F93" s="21"/>
+      <c r="G93" s="19"/>
       <c r="H93" s="19">
-        <f>(B93*G93)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I93" s="17" t="s">
-        <v>81</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I93" s="17"/>
       <c r="J93" s="20" t="s">
-        <v>216</v>
+        <v>305</v>
       </c>
       <c r="K93" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L93" s="2" t="s">
-        <v>319</v>
-      </c>
+      <c r="L93" s="3"/>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94" s="35">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B94" s="15">
         <v>1</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>304</v>
-      </c>
-      <c r="D94" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="E94" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>272</v>
-      </c>
-      <c r="G94" s="19">
-        <v>0.1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D94" s="17"/>
+      <c r="E94" s="21"/>
+      <c r="F94" s="21"/>
+      <c r="G94" s="19"/>
       <c r="H94" s="19">
-        <f t="shared" ref="H94:H97" si="4">(B94*G94)</f>
-        <v>0.1</v>
-      </c>
-      <c r="I94" s="17" t="s">
-        <v>82</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I94" s="17"/>
       <c r="J94" s="20" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="K94" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="L94" s="2"/>
+      <c r="L94" s="3"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="35">
+        <v>20</v>
+      </c>
+      <c r="B95" s="15">
+        <v>4</v>
+      </c>
+      <c r="C95" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D95" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="E95" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="F95" s="21" t="s">
+        <v>318</v>
+      </c>
+      <c r="G95" s="19">
+        <v>0.05</v>
+      </c>
+      <c r="H95" s="19">
+        <f>(B95*G95)</f>
+        <v>0.2</v>
+      </c>
+      <c r="I95" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="J95" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="K95" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A96" s="35">
+        <v>21</v>
+      </c>
+      <c r="B96" s="15">
+        <v>1</v>
+      </c>
+      <c r="C96" s="17" t="s">
+        <v>304</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="E96" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="F96" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="G96" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H96" s="19">
+        <f t="shared" ref="H96:H99" si="4">(B96*G96)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I96" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="J96" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="K96" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L96" s="2"/>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A97" s="35">
         <v>22</v>
       </c>
-      <c r="B95" s="15">
-        <v>1</v>
-      </c>
-      <c r="C95" s="17" t="s">
+      <c r="B97" s="15">
+        <v>1</v>
+      </c>
+      <c r="C97" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="D95" s="20" t="s">
+      <c r="D97" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="E95" s="21" t="s">
+      <c r="E97" s="21" t="s">
         <v>279</v>
       </c>
-      <c r="F95" s="21" t="s">
+      <c r="F97" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="G95" s="19">
+      <c r="G97" s="19">
         <v>0.11</v>
       </c>
-      <c r="H95" s="19">
+      <c r="H97" s="19">
         <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
-      <c r="I95" s="17" t="s">
+      <c r="I97" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="J95" s="20" t="s">
+      <c r="J97" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="K95" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="L95" s="2"/>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A96" s="35">
+      <c r="K97" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A98" s="35">
         <v>23</v>
       </c>
-      <c r="B96" s="15">
-        <v>1</v>
-      </c>
-      <c r="C96" s="17" t="s">
+      <c r="B98" s="15">
+        <v>1</v>
+      </c>
+      <c r="C98" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D96" s="15"/>
-      <c r="E96" s="15"/>
-      <c r="F96" s="15"/>
-      <c r="G96" s="19"/>
-      <c r="H96" s="19">
+      <c r="D98" s="15"/>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="19"/>
+      <c r="H98" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I96" s="27"/>
-      <c r="J96" s="20" t="s">
+      <c r="I98" s="27"/>
+      <c r="J98" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="K96" s="17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A97" s="35">
+      <c r="K98" s="17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A99" s="35">
         <v>24</v>
       </c>
-      <c r="B97" s="15">
-        <v>1</v>
-      </c>
-      <c r="C97" s="15"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="15"/>
-      <c r="F97" s="15"/>
-      <c r="G97" s="19"/>
-      <c r="H97" s="19">
+      <c r="B99" s="15">
+        <v>1</v>
+      </c>
+      <c r="C99" s="15"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="15"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="19"/>
+      <c r="H99" s="19">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I97" s="27"/>
-      <c r="J97" s="15"/>
-      <c r="K97" s="15"/>
-    </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-    </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I100" s="12"/>
-    </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H101" s="10" t="s">
+      <c r="I99" s="27"/>
+      <c r="J99" s="15"/>
+      <c r="K99" s="15"/>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A100" s="1"/>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I102" s="12"/>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H103" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="I101" s="5"/>
-    </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H102" s="9">
-        <f>SUM(H12:H70)</f>
-        <v>68.20999999999998</v>
-      </c>
-      <c r="I102" s="5"/>
-    </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H103" s="1"/>
-      <c r="I103" s="6"/>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H104" s="7" t="s">
+      <c r="I103" s="5"/>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H104" s="9">
+        <f>SUM(H12:H72)</f>
+        <v>71.089999999999989</v>
+      </c>
+      <c r="I104" s="5"/>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H105" s="1"/>
+      <c r="I105" s="6"/>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H106" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="I104" s="3"/>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H105" s="9">
-        <f>SUM(H74:H97)</f>
+      <c r="I106" s="3"/>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H107" s="9">
+        <f>SUM(H76:H99)</f>
         <v>5.4999999999999991</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H107" s="7" t="s">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H109" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H108" s="9">
-        <f>SUM(H102+H105)</f>
-        <v>73.70999999999998</v>
-      </c>
-    </row>
-    <row r="114" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H114" s="11"/>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H110" s="9">
+        <f>SUM(H104+H107)</f>
+        <v>76.589999999999989</v>
+      </c>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H116" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
BOM should be usable again for Rev2
</commit_message>
<xml_diff>
--- a/SPEX HAB2 BOM.xlsx
+++ b/SPEX HAB2 BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew\Desktop\SPEX_HAB_Mainboard_Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechStars\Documents\GitHub\SPEX_HAB_Mainboard_Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Turnkey" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$55</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="388">
   <si>
     <t>Description</t>
   </si>
@@ -87,27 +87,18 @@
     <t>U10</t>
   </si>
   <si>
-    <t>U11</t>
-  </si>
-  <si>
     <t>U12</t>
   </si>
   <si>
     <t>U2,U4,U5</t>
   </si>
   <si>
-    <t>MKL04Z32VLC4</t>
-  </si>
-  <si>
     <t>MMQA6V2T1G</t>
   </si>
   <si>
     <t>BME280</t>
   </si>
   <si>
-    <t>MCP2551-I/SN</t>
-  </si>
-  <si>
     <t>ST1480ABDR</t>
   </si>
   <si>
@@ -120,15 +111,9 @@
     <t>Y1</t>
   </si>
   <si>
-    <t>SW1</t>
-  </si>
-  <si>
     <t>TH1,TH2,TH3</t>
   </si>
   <si>
-    <t>Q1,Q2</t>
-  </si>
-  <si>
     <t>U105,U108</t>
   </si>
   <si>
@@ -198,9 +183,6 @@
     <t>33 ohm resistor</t>
   </si>
   <si>
-    <t>R2,R12,R13,R18,R29,R30,R31,R34,R35,R36,R37,R38,R109,R126,R130,R140,R141,R145</t>
-  </si>
-  <si>
     <t>10k ohm resistor</t>
   </si>
   <si>
@@ -217,9 +199,6 @@
   </si>
   <si>
     <t>4.7k ohm resistor</t>
-  </si>
-  <si>
-    <t>R32,R33</t>
   </si>
   <si>
     <t>120 ohm resistor</t>
@@ -484,12 +463,6 @@
     <t>2.5V precision voltage reference</t>
   </si>
   <si>
-    <t>579-MCP2551-I/SN</t>
-  </si>
-  <si>
-    <t>CAN Transceiver</t>
-  </si>
-  <si>
     <t>511-ST1480ABDR</t>
   </si>
   <si>
@@ -544,15 +517,6 @@
     <t>reset button</t>
   </si>
   <si>
-    <t>2N7002KT1G</t>
-  </si>
-  <si>
-    <t>863-2N7002KT1G</t>
-  </si>
-  <si>
-    <t>N channel mosfet</t>
-  </si>
-  <si>
     <t>BSS215P H6327</t>
   </si>
   <si>
@@ -1226,6 +1190,36 @@
   </si>
   <si>
     <t>LT6105IDCB#TRMPBFCT-ND</t>
+  </si>
+  <si>
+    <t>http://www.pjrc.com/store/ic_mkl02.html</t>
+  </si>
+  <si>
+    <t>MKL02z32VFG4</t>
+  </si>
+  <si>
+    <t>SW1,SW2</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R2,R12,R13,R18,R19,R20,R30,R31,R35,R36,R37,R38,R109,R126,R130,R140,R141,R145</t>
+  </si>
+  <si>
+    <t>TSOP-6</t>
+  </si>
+  <si>
+    <t>LQFP-64</t>
+  </si>
+  <si>
+    <t>MSOP-8</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>SOT-23-6</t>
   </si>
 </sst>
 </file>
@@ -1889,10 +1883,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R113"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1932,7 +1926,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2019,7 +2013,7 @@
         <v>12</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2040,32 +2034,37 @@
         <v>1</v>
       </c>
       <c r="B12" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>24</v>
+        <v>379</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19">
-        <v>6</v>
+        <v>6.8</v>
       </c>
       <c r="H12" s="19">
         <f>(B12*G12)</f>
-        <v>12</v>
+        <v>6.8</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="J12" s="20"/>
+        <v>126</v>
+      </c>
+      <c r="J12" s="20" t="s">
+        <v>357</v>
+      </c>
       <c r="K12" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
+      </c>
+      <c r="L12" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2073,34 +2072,36 @@
         <v>2</v>
       </c>
       <c r="B13" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
+        <f>(3*G98)</f>
+        <v>3</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F13" s="18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G13" s="19">
         <v>0.55000000000000004</v>
       </c>
       <c r="H13" s="19">
         <f t="shared" ref="H13:H19" si="0">(B13*G13)</f>
-        <v>3.3000000000000003</v>
+        <v>1.6500000000000001</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="J13" s="21"/>
+        <v>128</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>383</v>
+      </c>
       <c r="K13" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2108,34 +2109,36 @@
         <v>3</v>
       </c>
       <c r="B14" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G14" s="19">
         <v>7.07</v>
       </c>
       <c r="H14" s="19">
         <f t="shared" si="0"/>
-        <v>14.14</v>
+        <v>7.07</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="J14" s="23"/>
+        <v>125</v>
+      </c>
+      <c r="J14" s="23" t="s">
+        <v>384</v>
+      </c>
       <c r="K14" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -2143,34 +2146,36 @@
         <v>4</v>
       </c>
       <c r="B15" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G15" s="19">
         <v>0.48</v>
       </c>
       <c r="H15" s="19">
         <f>(B15*G15)</f>
-        <v>0.96</v>
+        <v>0.48</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="20"/>
+        <v>127</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>383</v>
+      </c>
       <c r="K15" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2178,34 +2183,36 @@
         <v>5</v>
       </c>
       <c r="B16" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G16" s="19">
         <v>1.22</v>
       </c>
       <c r="H16" s="19">
         <f t="shared" si="0"/>
-        <v>2.44</v>
+        <v>1.22</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="J16" s="20"/>
+        <v>129</v>
+      </c>
+      <c r="J16" s="20" t="s">
+        <v>385</v>
+      </c>
       <c r="K16" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2213,36 +2220,36 @@
         <v>6</v>
       </c>
       <c r="B17" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="G17" s="19">
         <v>5.66</v>
       </c>
       <c r="H17" s="19">
         <f t="shared" si="0"/>
-        <v>11.32</v>
+        <v>5.66</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2250,36 +2257,36 @@
         <v>7</v>
       </c>
       <c r="B18" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="G18" s="26">
         <v>6.21</v>
       </c>
       <c r="H18" s="19">
         <f t="shared" si="0"/>
-        <v>12.42</v>
+        <v>6.21</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2287,603 +2294,614 @@
         <v>8</v>
       </c>
       <c r="B19" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F19" s="27" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="G19" s="28">
         <v>2.12</v>
       </c>
       <c r="H19" s="19">
         <f t="shared" si="0"/>
-        <v>4.24</v>
+        <v>2.12</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B20" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>126</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>27</v>
+        <v>124</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G20" s="19">
-        <v>1.1200000000000001</v>
+        <v>1.4</v>
       </c>
       <c r="H20" s="19">
-        <f t="shared" ref="H20:H29" si="1">(B20*G20)</f>
-        <v>2.2400000000000002</v>
+        <f t="shared" ref="H20:H27" si="1">(B20*G20)</f>
+        <v>1.4</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="J20" s="20"/>
+        <v>140</v>
+      </c>
+      <c r="J20" s="20" t="s">
+        <v>272</v>
+      </c>
       <c r="K20" s="17" t="s">
-        <v>182</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B21" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>22</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>28</v>
+        <v>138</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>136</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="G21" s="19">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="H21" s="19">
         <f t="shared" si="1"/>
-        <v>2.8</v>
+        <v>0.8</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="J21" s="20" t="s">
-        <v>284</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="J21" s="20"/>
       <c r="K21" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>29</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>27</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>142</v>
       </c>
       <c r="G22" s="19">
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="H22" s="19">
         <f t="shared" si="1"/>
-        <v>1.6</v>
+        <v>4</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="J22" s="20"/>
+        <v>143</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>386</v>
+      </c>
       <c r="K22" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="E23" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>151</v>
+        <v>88</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="G23" s="19">
-        <v>4</v>
+        <v>1.45</v>
       </c>
       <c r="H23" s="19">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>2.9</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="J23" s="20"/>
+        <v>147</v>
+      </c>
+      <c r="J23" s="20" t="s">
+        <v>387</v>
+      </c>
       <c r="K23" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B24" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="G24" s="19">
-        <v>1.45</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="G24" s="28">
+        <v>0.72</v>
       </c>
       <c r="H24" s="19">
         <f t="shared" si="1"/>
-        <v>5.8</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>156</v>
+        <v>0.72</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>150</v>
       </c>
       <c r="J24" s="20"/>
       <c r="K24" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C25" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="G25" s="28">
-        <v>0.72</v>
+      <c r="C25" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>310</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="F25" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="G25" s="19">
+        <v>0.42</v>
       </c>
       <c r="H25" s="19">
         <f t="shared" si="1"/>
-        <v>1.44</v>
-      </c>
-      <c r="I25" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="J25" s="20"/>
+        <v>0.84</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="J25" s="20" t="s">
+        <v>311</v>
+      </c>
       <c r="K25" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B26" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(3*G98)</f>
+        <v>3</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>322</v>
-      </c>
-      <c r="E26" s="17" t="s">
-        <v>320</v>
+        <v>306</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>304</v>
       </c>
       <c r="F26" s="29" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="G26" s="19">
-        <v>0.42</v>
+        <v>0.26</v>
       </c>
       <c r="H26" s="19">
         <f t="shared" si="1"/>
-        <v>0.84</v>
+        <v>0.78</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B27" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="25" t="s">
-        <v>318</v>
+        <v>31</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>155</v>
       </c>
       <c r="E27" s="15" t="s">
-        <v>316</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>317</v>
+        <v>153</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="G27" s="19">
-        <v>0.26</v>
+        <v>0.46</v>
       </c>
       <c r="H27" s="19">
         <f t="shared" si="1"/>
-        <v>1.56</v>
+        <v>0.46</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" s="20" t="s">
-        <v>319</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="J27" s="20"/>
       <c r="K27" s="17" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B28" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(3*G98)</f>
+        <v>3</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="17" t="s">
         <v>162</v>
       </c>
-      <c r="F28" s="29" t="s">
-        <v>163</v>
+      <c r="E28" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>158</v>
       </c>
       <c r="G28" s="19">
-        <v>0.2</v>
+        <v>0.52</v>
       </c>
       <c r="H28" s="19">
-        <f t="shared" si="1"/>
-        <v>0.8</v>
+        <f t="shared" ref="H28:H51" si="2">(B28*G28)</f>
+        <v>1.56</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="J28" s="20"/>
       <c r="K28" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B29" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>167</v>
+        <v>327</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>165</v>
+        <v>323</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>166</v>
+        <v>324</v>
       </c>
       <c r="G29" s="19">
-        <v>0.46</v>
+        <v>0.37</v>
       </c>
       <c r="H29" s="19">
-        <f t="shared" si="1"/>
-        <v>0.92</v>
+        <f t="shared" si="2"/>
+        <v>0.74</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="J29" s="20"/>
+        <v>325</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>326</v>
+      </c>
       <c r="K29" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B30" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>169</v>
+        <v>162</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>160</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="G30" s="19">
         <v>0.52</v>
       </c>
       <c r="H30" s="19">
-        <f t="shared" ref="H30:H53" si="2">(B30*G30)</f>
-        <v>3.12</v>
+        <f t="shared" si="2"/>
+        <v>0.52</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="J30" s="20"/>
       <c r="K30" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B31" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>339</v>
+        <v>111</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>335</v>
+        <v>318</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="G31" s="19">
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="H31" s="19">
         <f t="shared" si="2"/>
-        <v>1.48</v>
+        <v>0.1</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
+      </c>
+      <c r="L31" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B32" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="G32" s="19">
-        <v>0.52</v>
+        <v>0.13</v>
       </c>
       <c r="H32" s="19">
         <f t="shared" si="2"/>
-        <v>1.04</v>
+        <v>0.13</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="J32" s="20"/>
+        <v>167</v>
+      </c>
+      <c r="J32" s="20" t="s">
+        <v>168</v>
+      </c>
       <c r="K32" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
+      </c>
+      <c r="L32" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B33" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>118</v>
+        <v>298</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>330</v>
+        <v>296</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>331</v>
+        <v>297</v>
       </c>
       <c r="G33" s="19">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="H33" s="19">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>333</v>
+        <v>218</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>334</v>
+        <v>168</v>
       </c>
       <c r="K33" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L33" t="s">
-        <v>332</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B34" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>177</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>299</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>298</v>
+      </c>
+      <c r="E34" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>301</v>
       </c>
       <c r="G34" s="19">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="H34" s="19">
         <f t="shared" si="2"/>
-        <v>0.26</v>
+        <v>0.1</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>179</v>
+        <v>302</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L34" t="s">
-        <v>181</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A35" s="14">
-        <v>25</v>
+      <c r="A35" s="33">
+        <v>28</v>
       </c>
       <c r="B35" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C35" s="25" t="s">
-        <v>42</v>
+      <c r="C35" s="17" t="s">
+        <v>38</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>310</v>
+        <v>192</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>308</v>
+        <v>39</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>309</v>
+        <v>171</v>
       </c>
       <c r="G35" s="19">
         <v>0.15</v>
@@ -2893,200 +2911,201 @@
         <v>0.3</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>230</v>
+        <v>172</v>
       </c>
       <c r="J35" s="20" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="K35" s="17" t="s">
-        <v>182</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L35" s="2"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="14">
-        <v>26</v>
+      <c r="A36" s="33">
+        <v>29</v>
       </c>
       <c r="B36" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C36" s="30" t="s">
-        <v>311</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="E36" s="25" t="s">
-        <v>312</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>313</v>
+      <c r="C36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>333</v>
       </c>
       <c r="G36" s="19">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="2"/>
-        <v>0.2</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="J36" s="20" t="s">
-        <v>180</v>
-      </c>
+        <v>0.38</v>
+      </c>
+      <c r="I36" s="17"/>
+      <c r="J36" s="20"/>
       <c r="K36" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L36" t="s">
-        <v>315</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L36" s="3"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="33">
-        <v>28</v>
+      <c r="A37" s="34">
+        <v>30</v>
       </c>
       <c r="B37" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>204</v>
+        <v>111</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>183</v>
+        <v>335</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>334</v>
       </c>
       <c r="G37" s="19">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H37" s="19">
         <f t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="I37" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="J37" s="20" t="s">
-        <v>185</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I37" s="15"/>
+      <c r="J37" s="20"/>
       <c r="K37" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L37" s="2"/>
+        <v>170</v>
+      </c>
+      <c r="L37" s="3"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B38" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>45</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>328</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>339</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>344</v>
+        <v>338</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>336</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="G38" s="19">
-        <v>0.19</v>
+        <v>0.38</v>
       </c>
       <c r="H38" s="19">
-        <f t="shared" si="2"/>
-        <v>0.76</v>
-      </c>
-      <c r="I38" s="17"/>
+        <f>(B38*G38)</f>
+        <v>0.38</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>330</v>
+      </c>
       <c r="J38" s="20"/>
       <c r="K38" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="34">
-        <v>30</v>
+      <c r="A39" s="33">
+        <v>32</v>
       </c>
       <c r="B39" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>46</v>
+        <v>329</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>118</v>
+        <v>340</v>
       </c>
       <c r="E39" s="15" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G39" s="19">
-        <v>0</v>
+        <v>0.48</v>
       </c>
       <c r="H39" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I39" s="15"/>
-      <c r="J39" s="20"/>
+        <v>0.48</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="J39" s="20" t="s">
+        <v>342</v>
+      </c>
       <c r="K39" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="33">
-        <v>31</v>
+      <c r="A40" s="34">
+        <v>33</v>
       </c>
       <c r="B40" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>340</v>
+        <v>42</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>350</v>
+        <v>327</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>348</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>349</v>
+        <v>343</v>
+      </c>
+      <c r="F40" s="15" t="s">
+        <v>344</v>
       </c>
       <c r="G40" s="19">
-        <v>0.38</v>
+        <v>0.34</v>
       </c>
       <c r="H40" s="19">
-        <f>(B40*G40)</f>
-        <v>0.76</v>
+        <f t="shared" si="2"/>
+        <v>0.34</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="J40" s="20"/>
       <c r="K40" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="1"/>
@@ -3094,449 +3113,455 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="33">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B41" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>341</v>
+        <v>43</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>352</v>
+        <v>232</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>351</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>353</v>
+        <v>314</v>
+      </c>
+      <c r="F41" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="G41" s="19">
-        <v>0.48</v>
+        <v>0.46</v>
       </c>
       <c r="H41" s="19">
         <f t="shared" si="2"/>
-        <v>0.96</v>
+        <v>0.46</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="J41" s="20" t="s">
-        <v>354</v>
+        <v>317</v>
       </c>
       <c r="K41" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="34">
-        <v>33</v>
+      <c r="A42" s="33">
+        <v>35</v>
       </c>
       <c r="B42" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>47</v>
+      <c r="C42" s="27" t="s">
+        <v>44</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>339</v>
+        <v>194</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>355</v>
+        <v>193</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>356</v>
+        <v>175</v>
       </c>
       <c r="G42" s="19">
-        <v>0.34</v>
+        <v>1.43</v>
       </c>
       <c r="H42" s="19">
         <f t="shared" si="2"/>
-        <v>0.68</v>
+        <v>2.86</v>
       </c>
       <c r="I42" s="17" t="s">
-        <v>357</v>
-      </c>
-      <c r="J42" s="20"/>
+        <v>176</v>
+      </c>
+      <c r="J42" s="21"/>
       <c r="K42" s="17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
+      <c r="R42" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="33">
-        <v>34</v>
+      <c r="A43" s="34">
+        <v>36</v>
       </c>
       <c r="B43" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C43" s="17" t="s">
-        <v>48</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>326</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>327</v>
+        <v>346</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>347</v>
       </c>
       <c r="G43" s="19">
-        <v>0.46</v>
+        <v>0.97</v>
       </c>
       <c r="H43" s="19">
         <f t="shared" si="2"/>
-        <v>0.92</v>
+        <v>0.97</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>328</v>
-      </c>
-      <c r="J43" s="20" t="s">
-        <v>329</v>
-      </c>
+        <v>348</v>
+      </c>
+      <c r="J43" s="20"/>
       <c r="K43" s="17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L43" s="3"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="33">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B44" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F44" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="G44" s="19">
-        <v>1.43</v>
-      </c>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="17"/>
+      <c r="E44" s="15"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="19"/>
       <c r="H44" s="19">
         <f t="shared" si="2"/>
-        <v>5.72</v>
-      </c>
-      <c r="I44" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="J44" s="21"/>
-      <c r="K44" s="17" t="s">
-        <v>189</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="17"/>
       <c r="L44" s="3"/>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
-      <c r="R44" s="2" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="34">
-        <v>36</v>
+      <c r="A45" s="33">
+        <v>38</v>
       </c>
       <c r="B45" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(4*G98)</f>
+        <v>4</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>358</v>
-      </c>
-      <c r="F45" s="17" t="s">
-        <v>359</v>
+        <v>47</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" s="17"/>
+      <c r="F45" s="15" t="s">
+        <v>182</v>
       </c>
       <c r="G45" s="19">
-        <v>0.97</v>
+        <v>1.5</v>
       </c>
       <c r="H45" s="19">
         <f t="shared" si="2"/>
-        <v>1.94</v>
-      </c>
-      <c r="I45" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="J45" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="I45" s="32" t="s">
+        <v>183</v>
+      </c>
+      <c r="J45" s="36" t="s">
+        <v>271</v>
+      </c>
       <c r="K45" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="L45" s="3"/>
+        <v>177</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="33">
-        <v>37</v>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A46" s="34">
+        <v>39</v>
       </c>
       <c r="B46" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C46" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D46" s="17"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="17"/>
-      <c r="G46" s="19"/>
+        <f>(7*G98)</f>
+        <v>7</v>
+      </c>
+      <c r="C46" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="G46" s="19">
+        <v>0.72</v>
+      </c>
       <c r="H46" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I46" s="17"/>
-      <c r="J46" s="20"/>
-      <c r="K46" s="17"/>
+        <v>5.04</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J46" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="K46" s="17" t="s">
+        <v>177</v>
+      </c>
       <c r="L46" s="3"/>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="33">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B47" s="15">
-        <f>(4*G100)</f>
-        <v>8</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="E47" s="17"/>
+        <f>(4*G98)</f>
+        <v>4</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>199</v>
+      </c>
       <c r="F47" s="15" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="G47" s="19">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="H47" s="19">
         <f t="shared" si="2"/>
-        <v>12</v>
-      </c>
-      <c r="I47" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="J47" s="36" t="s">
-        <v>283</v>
+        <v>0.4</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="L47" s="3" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
+      <c r="R47" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="34">
-        <v>39</v>
+      <c r="A48" s="33">
+        <v>41</v>
       </c>
       <c r="B48" s="15">
-        <f>(7*G100)</f>
-        <v>14</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>98</v>
+        <f>(18*G98)</f>
+        <v>18</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>200</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>191</v>
+        <v>203</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>204</v>
       </c>
       <c r="G48" s="19">
-        <v>0.72</v>
+        <v>0.1</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>10.08</v>
+        <v>1.8</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>283</v>
+        <v>53</v>
+      </c>
+      <c r="J48" s="20" t="s">
+        <v>168</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="L48" s="3"/>
+        <v>170</v>
+      </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
+      <c r="R48" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="33">
-        <v>40</v>
+      <c r="A49" s="34">
+        <v>42</v>
       </c>
       <c r="B49" s="15">
-        <f>(4*G100)</f>
-        <v>8</v>
-      </c>
-      <c r="C49" s="17" t="s">
-        <v>54</v>
+        <f>(2*G98)</f>
+        <v>2</v>
+      </c>
+      <c r="C49" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G49" s="19">
         <v>0.1</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L49" s="3" t="s">
-        <v>214</v>
+        <v>170</v>
       </c>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
-      <c r="R49" s="2" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="33">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B50" s="15">
-        <f>(18*G100)</f>
-        <v>36</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>58</v>
+        <f>(3*G98)</f>
+        <v>3</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>54</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="F50" s="16" t="s">
-        <v>216</v>
+        <v>210</v>
+      </c>
+      <c r="F50" s="15" t="s">
+        <v>208</v>
       </c>
       <c r="G50" s="19">
         <v>0.1</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>3.6</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>59</v>
+        <v>211</v>
       </c>
       <c r="J50" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
+      </c>
+      <c r="L50" t="s">
+        <v>212</v>
       </c>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
-      <c r="R50" s="2" t="s">
-        <v>213</v>
-      </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="34">
-        <v>42</v>
+      <c r="A51" s="33">
+        <v>44</v>
       </c>
       <c r="B51" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>56</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>55</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G51" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H51" s="19">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>0.08</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J51" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K51" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
+      </c>
+      <c r="L51" t="s">
+        <v>217</v>
       </c>
       <c r="M51" s="1"/>
       <c r="N51" s="1"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="33">
-        <v>43</v>
+      <c r="A52" s="34">
+        <v>45</v>
       </c>
       <c r="B52" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>60</v>
+        <f>(5*G98)</f>
+        <v>5</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="E52" s="15" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="F52" s="15" t="s">
         <v>220</v>
@@ -3545,1276 +3570,1270 @@
         <v>0.1</v>
       </c>
       <c r="H52" s="19">
-        <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
+        <f t="shared" ref="H52:H89" si="3">(B52*G52)</f>
+        <v>0.5</v>
       </c>
       <c r="I52" s="17" t="s">
-        <v>223</v>
+        <v>58</v>
       </c>
       <c r="J52" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K52" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L52" t="s">
-        <v>224</v>
-      </c>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="R52" s="2" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="33">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B53" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>61</v>
+        <v>381</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>228</v>
+        <v>215</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>221</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G53" s="19">
         <v>0.08</v>
       </c>
       <c r="H53" s="19">
-        <f t="shared" si="2"/>
-        <v>0.16</v>
+        <f t="shared" si="3"/>
+        <v>0.08</v>
       </c>
       <c r="I53" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J53" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K53" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L53" t="s">
-        <v>229</v>
-      </c>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="34">
-        <v>45</v>
+      <c r="A54" s="33">
+        <v>47</v>
       </c>
       <c r="B54" s="15">
-        <f>(5*G100)</f>
-        <v>10</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>231</v>
+        <v>200</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>223</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G54" s="19">
         <v>0.1</v>
       </c>
       <c r="H54" s="19">
-        <f t="shared" ref="H54:H91" si="3">(B54*G54)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0.2</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="J54" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L54" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="R54" s="2" t="s">
-        <v>213</v>
+        <v>170</v>
+      </c>
+      <c r="L54" s="31" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="33">
-        <v>46</v>
+      <c r="A55" s="34">
+        <v>48</v>
       </c>
       <c r="B55" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D55" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E55" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="F55" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="E55" s="17" t="s">
-        <v>233</v>
-      </c>
-      <c r="F55" s="15" t="s">
-        <v>234</v>
-      </c>
       <c r="G55" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H55" s="19">
         <f t="shared" si="3"/>
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J55" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>229</v>
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="33">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B56" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>235</v>
+        <v>200</v>
+      </c>
+      <c r="E56" s="15" t="s">
+        <v>229</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="G56" s="19">
         <v>0.1</v>
       </c>
       <c r="H56" s="19">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="J56" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L56" s="31" t="s">
-        <v>237</v>
+        <v>170</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="34">
-        <v>48</v>
+      <c r="A57" s="33">
+        <v>50</v>
       </c>
       <c r="B57" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>239</v>
+        <v>66</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>231</v>
       </c>
       <c r="G57" s="19">
         <v>0.1</v>
       </c>
       <c r="H57" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="J57" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L57" s="3" t="s">
-        <v>214</v>
+        <v>170</v>
+      </c>
+      <c r="L57" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="33">
-        <v>49</v>
+      <c r="A58" s="34">
+        <v>51</v>
       </c>
       <c r="B58" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G58" s="19">
         <v>0.1</v>
       </c>
       <c r="H58" s="19">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="33">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B59" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>244</v>
-      </c>
-      <c r="E59" s="25" t="s">
-        <v>242</v>
-      </c>
-      <c r="F59" s="17" t="s">
-        <v>243</v>
+        <v>70</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>238</v>
       </c>
       <c r="G59" s="19">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.09</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J59" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L59" t="s">
-        <v>245</v>
+        <v>170</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="34">
-        <v>51</v>
+      <c r="A60" s="33">
+        <v>53</v>
       </c>
       <c r="B60" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(8*G98)</f>
+        <v>8</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D60" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>246</v>
-      </c>
-      <c r="F60" s="15" t="s">
-        <v>247</v>
+        <v>72</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="F60" s="21" t="s">
+        <v>244</v>
       </c>
       <c r="G60" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.64</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J60" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L60" s="3" t="s">
-        <v>214</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L60" s="3"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="33">
-        <v>52</v>
+      <c r="A61" s="34">
+        <v>54</v>
       </c>
       <c r="B61" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D61" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>248</v>
-      </c>
-      <c r="F61" s="15" t="s">
-        <v>250</v>
+        <v>73</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>251</v>
+      </c>
+      <c r="F61" s="21" t="s">
+        <v>252</v>
       </c>
       <c r="G61" s="19">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="3"/>
-        <v>0.18</v>
+        <v>0.1</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J61" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K61" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L61" s="3" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="33">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B62" s="15">
-        <f>(8*G100)</f>
-        <v>16</v>
+        <f>(8*G98)</f>
+        <v>8</v>
       </c>
       <c r="C62" s="17" t="s">
-        <v>79</v>
+        <v>249</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="G62" s="19">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="3"/>
-        <v>1.28</v>
+        <v>0.32</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>81</v>
+        <v>250</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K62" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L62" s="3"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="34">
-        <v>54</v>
+      <c r="A63" s="33">
+        <v>56</v>
       </c>
       <c r="B63" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>80</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>245</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="E63" s="20" t="s">
-        <v>263</v>
+        <v>240</v>
+      </c>
+      <c r="E63" s="21" t="s">
+        <v>246</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="G63" s="19">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J63" s="20" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="K63" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>266</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="33">
-        <v>55</v>
+      <c r="A64" s="34">
+        <v>57</v>
       </c>
       <c r="B64" s="15">
-        <f>(8*G100)</f>
-        <v>16</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C64" s="17" t="s">
-        <v>261</v>
+        <v>77</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="G64" s="19">
         <v>0.04</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="3"/>
-        <v>0.64</v>
+        <v>0.04</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J64" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K64" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L64" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>258</v>
+      </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="33">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B65" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C65" s="32" t="s">
-        <v>257</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G65" s="19">
-        <v>0.02</v>
+        <v>0.11</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J65" s="20" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="K65" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L65" s="3" t="s">
-        <v>260</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L65" s="3"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="34">
-        <v>57</v>
+      <c r="A66" s="33">
+        <v>59</v>
       </c>
       <c r="B66" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>268</v>
+        <v>374</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>269</v>
+        <v>375</v>
       </c>
       <c r="G66" s="19">
-        <v>0.04</v>
+        <v>0.2</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="3"/>
-        <v>0.08</v>
+        <v>0.4</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>267</v>
+        <v>80</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="K66" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L66" s="3" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="33">
-        <v>58</v>
+      <c r="A67" s="34">
+        <v>60</v>
       </c>
       <c r="B67" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="G67" s="19">
-        <v>0.11</v>
+        <v>0.5</v>
       </c>
       <c r="H67" s="19">
         <f t="shared" si="3"/>
-        <v>0.22</v>
+        <v>1</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L67" s="3"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="33">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B68" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>386</v>
+        <v>265</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>387</v>
+        <v>266</v>
       </c>
       <c r="G68" s="19">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="3"/>
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I68" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="J68" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="K68" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="L68" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A69" s="33">
+        <v>62</v>
+      </c>
+      <c r="B69" s="15">
+        <f>(3*G98)</f>
+        <v>3</v>
+      </c>
+      <c r="C69" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="J68" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="K68" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L68" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="34">
-        <v>60</v>
-      </c>
-      <c r="B69" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>93</v>
-      </c>
       <c r="D69" s="20" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="G69" s="19">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="J69" s="20" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="K69" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L69" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="L69" s="3" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="33">
-        <v>61</v>
+      <c r="A70" s="34">
+        <v>63</v>
       </c>
       <c r="B70" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
-      </c>
-      <c r="C70" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="E70" s="21" t="s">
-        <v>277</v>
-      </c>
-      <c r="F70" s="21" t="s">
-        <v>278</v>
+        <f>(7*G98)</f>
+        <v>7</v>
+      </c>
+      <c r="C70" s="17"/>
+      <c r="D70" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E70" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="F70" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="G70" s="19">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>2.17</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="J70" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="K70" s="17" t="s">
-        <v>182</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="J70" s="20"/>
+      <c r="K70" s="17"/>
       <c r="L70" s="3" t="s">
-        <v>273</v>
+        <v>186</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A71" s="33">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B71" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
-      </c>
-      <c r="C71" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D71" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="E71" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="F71" s="21" t="s">
-        <v>280</v>
+        <f>(14*G98)</f>
+        <v>14</v>
+      </c>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E71" s="15">
+        <v>1722533123</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="G71" s="19">
-        <v>0.1</v>
+        <v>0.152</v>
       </c>
       <c r="H71" s="19">
         <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <v>2.1280000000000001</v>
       </c>
       <c r="I71" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="J71" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="K71" s="17" t="s">
-        <v>182</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="J71" s="20"/>
+      <c r="K71" s="17"/>
       <c r="L71" s="3" t="s">
-        <v>282</v>
+        <v>190</v>
+      </c>
+      <c r="R71" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="34">
-        <v>63</v>
-      </c>
-      <c r="B72" s="15">
-        <f>(7*G100)</f>
-        <v>14</v>
-      </c>
-      <c r="C72" s="17"/>
-      <c r="D72" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E72" s="15" t="s">
-        <v>197</v>
-      </c>
-      <c r="F72" s="15" t="s">
-        <v>196</v>
-      </c>
-      <c r="G72" s="19">
-        <v>0.31</v>
-      </c>
-      <c r="H72" s="19">
-        <f t="shared" si="3"/>
-        <v>4.34</v>
-      </c>
-      <c r="I72" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="J72" s="20"/>
-      <c r="K72" s="17"/>
-      <c r="L72" s="3" t="s">
-        <v>198</v>
-      </c>
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="40"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="3"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A73" s="33">
-        <v>64</v>
+      <c r="A73" s="35">
+        <v>1</v>
       </c>
       <c r="B73" s="15">
-        <f>(14*G100)</f>
-        <v>28</v>
-      </c>
-      <c r="C73" s="17"/>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>15</v>
+      </c>
       <c r="D73" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E73" s="15">
-        <v>1722533123</v>
+        <v>124</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>203</v>
+        <v>135</v>
       </c>
       <c r="G73" s="19">
-        <v>0.152</v>
+        <v>1.4</v>
       </c>
       <c r="H73" s="19">
         <f t="shared" si="3"/>
-        <v>4.2560000000000002</v>
+        <v>1.4</v>
       </c>
       <c r="I73" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="J73" s="20"/>
-      <c r="K73" s="17"/>
-      <c r="L73" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="R73" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="37"/>
-      <c r="B74" s="37"/>
-      <c r="C74" s="38"/>
-      <c r="D74" s="38"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="37"/>
-      <c r="G74" s="39"/>
-      <c r="H74" s="39"/>
-      <c r="I74" s="38"/>
-      <c r="J74" s="40"/>
-      <c r="K74" s="37"/>
+        <v>140</v>
+      </c>
+      <c r="J73" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="K73" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="35">
+        <v>2</v>
+      </c>
+      <c r="B74" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="E74" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="F74" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="G74" s="19">
+        <v>0.64</v>
+      </c>
+      <c r="H74" s="19">
+        <f t="shared" si="3"/>
+        <v>0.64</v>
+      </c>
+      <c r="I74" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="J74" s="20" t="s">
+        <v>361</v>
+      </c>
+      <c r="K74" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="L74" s="3"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B75" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>28</v>
+        <v>354</v>
       </c>
       <c r="F75" s="15" t="s">
-        <v>144</v>
+        <v>355</v>
       </c>
       <c r="G75" s="19">
-        <v>1.4</v>
+        <v>1.24</v>
       </c>
       <c r="H75" s="19">
         <f t="shared" si="3"/>
-        <v>2.8</v>
+        <v>1.24</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>149</v>
+        <v>356</v>
       </c>
       <c r="J75" s="20" t="s">
-        <v>284</v>
+        <v>357</v>
       </c>
       <c r="K75" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B76" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D76" s="17" t="s">
-        <v>374</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>370</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>371</v>
+        <v>94</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>120</v>
       </c>
       <c r="G76" s="19">
-        <v>0.64</v>
+        <v>5.66</v>
       </c>
       <c r="H76" s="19">
-        <f t="shared" si="3"/>
-        <v>1.28</v>
+        <f>(B76*G76)</f>
+        <v>5.66</v>
       </c>
       <c r="I76" s="17" t="s">
-        <v>372</v>
+        <v>130</v>
       </c>
       <c r="J76" s="20" t="s">
-        <v>373</v>
+        <v>350</v>
       </c>
       <c r="K76" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L76" s="3"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="35">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B77" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>122</v>
+        <v>312</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>366</v>
+        <v>376</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>367</v>
+        <v>377</v>
       </c>
       <c r="G77" s="19">
-        <v>1.24</v>
+        <v>2.84</v>
       </c>
       <c r="H77" s="19">
         <f t="shared" si="3"/>
-        <v>2.48</v>
+        <v>2.84</v>
       </c>
       <c r="I77" s="17" t="s">
-        <v>368</v>
+        <v>273</v>
       </c>
       <c r="J77" s="20" t="s">
-        <v>369</v>
+        <v>274</v>
       </c>
       <c r="K77" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L77" s="3"/>
+      <c r="R77" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="35">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B78" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D78" s="25" t="s">
-        <v>130</v>
-      </c>
-      <c r="E78" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" s="17" t="s">
-        <v>127</v>
+        <v>95</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="F78" s="15" t="s">
+        <v>275</v>
       </c>
       <c r="G78" s="19">
-        <v>5.66</v>
+        <v>0.86</v>
       </c>
       <c r="H78" s="19">
-        <f>(B78*G78)</f>
-        <v>11.32</v>
+        <f t="shared" si="3"/>
+        <v>0.86</v>
       </c>
       <c r="I78" s="17" t="s">
-        <v>137</v>
+        <v>276</v>
       </c>
       <c r="J78" s="20" t="s">
-        <v>362</v>
+        <v>277</v>
       </c>
       <c r="K78" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L78" s="3"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="35">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B79" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="E79" s="17" t="s">
-        <v>388</v>
+        <v>298</v>
+      </c>
+      <c r="E79" s="15" t="s">
+        <v>296</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>389</v>
+        <v>297</v>
       </c>
       <c r="G79" s="19">
-        <v>2.84</v>
+        <v>0.15</v>
       </c>
       <c r="H79" s="19">
         <f t="shared" si="3"/>
-        <v>5.68</v>
+        <v>0.15</v>
       </c>
       <c r="I79" s="17" t="s">
-        <v>285</v>
+        <v>218</v>
       </c>
       <c r="J79" s="20" t="s">
-        <v>286</v>
+        <v>168</v>
       </c>
       <c r="K79" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L79" s="3"/>
-      <c r="R79" s="2" t="s">
-        <v>186</v>
-      </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="35">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B80" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C80" s="17" t="s">
-        <v>102</v>
+        <v>45</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>325</v>
+        <v>91</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F80" s="15" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="G80" s="19">
-        <v>0.86</v>
+        <v>0.67</v>
       </c>
       <c r="H80" s="19">
         <f t="shared" si="3"/>
-        <v>1.72</v>
+        <v>0.67</v>
       </c>
       <c r="I80" s="17" t="s">
-        <v>288</v>
+        <v>97</v>
       </c>
       <c r="J80" s="20" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="K80" s="17" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="L80" s="3"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="35">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B81" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D81" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="E81" s="15" t="s">
-        <v>308</v>
-      </c>
-      <c r="F81" s="15" t="s">
-        <v>309</v>
-      </c>
-      <c r="G81" s="19">
-        <v>0.15</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D81" s="17"/>
+      <c r="E81" s="15"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="19"/>
       <c r="H81" s="19">
         <f t="shared" si="3"/>
-        <v>0.3</v>
-      </c>
-      <c r="I81" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="J81" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="K81" s="17" t="s">
-        <v>182</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I81" s="17"/>
+      <c r="J81" s="20"/>
+      <c r="K81" s="15"/>
       <c r="L81" s="3"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="35">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B82" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E82" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="G82" s="19">
-        <v>0.67</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D82" s="17"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="19"/>
       <c r="H82" s="19">
         <f t="shared" si="3"/>
-        <v>1.34</v>
-      </c>
-      <c r="I82" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>283</v>
-      </c>
-      <c r="K82" s="17" t="s">
-        <v>189</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J82" s="20"/>
+      <c r="K82" s="15"/>
       <c r="L82" s="3"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="35">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B83" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D83" s="17"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="19"/>
+        <v>99</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E83" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F83" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="G83" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H83" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I83" s="17"/>
-      <c r="J83" s="20"/>
-      <c r="K83" s="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="I83" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="J83" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="K83" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="L83" s="3"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="35">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B84" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D84" s="17"/>
-      <c r="F84" s="15"/>
-      <c r="G84" s="19"/>
+        <v>101</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="F84" s="15" t="s">
+        <v>283</v>
+      </c>
+      <c r="G84" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H84" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J84" s="20"/>
-      <c r="K84" s="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="I84" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="J84" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="K84" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="L84" s="3"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="35">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B85" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(3*G98)</f>
+        <v>3</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>106</v>
+        <v>352</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="G85" s="19">
         <v>0.1</v>
       </c>
       <c r="H85" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I85" s="17" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J85" s="20" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="K85" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L85" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="L85" s="3" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="35">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B86" s="15">
-        <f>(1*G100)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G86" s="19">
         <v>0.1</v>
@@ -4824,447 +4843,369 @@
         <v>0.2</v>
       </c>
       <c r="I86" s="17" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="J86" s="20" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="K86" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L86" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="L86" s="3" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="35">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B87" s="15">
-        <f>(3*G100)</f>
-        <v>6</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>364</v>
+        <v>105</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="E87" s="15" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="F87" s="15" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G87" s="19">
         <v>0.1</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="3"/>
-        <v>0.60000000000000009</v>
+        <v>0.1</v>
       </c>
       <c r="I87" s="17" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="J87" s="20" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="K87" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L87" s="3" t="s">
-        <v>229</v>
+        <v>292</v>
       </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="35">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B88" s="15">
-        <f>(2*G100)</f>
-        <v>4</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E88" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="F88" s="15" t="s">
-        <v>299</v>
+        <v>365</v>
+      </c>
+      <c r="E88" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="F88" s="21" t="s">
+        <v>363</v>
       </c>
       <c r="G88" s="19">
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="H88" s="19">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="I88" s="17" t="s">
-        <v>64</v>
+        <v>353</v>
       </c>
       <c r="J88" s="20" t="s">
-        <v>208</v>
+        <v>281</v>
       </c>
       <c r="K88" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L88" s="3" t="s">
-        <v>214</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L88" s="3"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="35">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B89" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="E89" s="15" t="s">
-        <v>302</v>
-      </c>
-      <c r="F89" s="15" t="s">
-        <v>303</v>
+        <v>215</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="F89" s="21" t="s">
+        <v>367</v>
       </c>
       <c r="G89" s="19">
         <v>0.1</v>
       </c>
       <c r="H89" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I89" s="17" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="J89" s="20" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="K89" s="17" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="L89" s="3" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="35">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B90" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(5*G98)</f>
+        <v>5</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>113</v>
+        <v>372</v>
       </c>
       <c r="D90" s="17" t="s">
-        <v>377</v>
-      </c>
-      <c r="E90" s="21" t="s">
-        <v>376</v>
+        <v>240</v>
+      </c>
+      <c r="E90" s="20" t="s">
+        <v>293</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>375</v>
+        <v>294</v>
       </c>
       <c r="G90" s="19">
-        <v>0.37</v>
+        <v>0.05</v>
       </c>
       <c r="H90" s="19">
-        <f t="shared" si="3"/>
-        <v>0.74</v>
+        <f>(B90*G90)</f>
+        <v>0.25</v>
       </c>
       <c r="I90" s="17" t="s">
-        <v>365</v>
+        <v>74</v>
       </c>
       <c r="J90" s="20" t="s">
-        <v>293</v>
+        <v>196</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L90" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="35">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B91" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D91" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="E91" s="21" t="s">
-        <v>378</v>
+        <v>280</v>
+      </c>
+      <c r="D91" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E91" s="20" t="s">
+        <v>251</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>379</v>
+        <v>252</v>
       </c>
       <c r="G91" s="19">
         <v>0.1</v>
       </c>
       <c r="H91" s="19">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
+        <f t="shared" ref="H91:H94" si="4">(B91*G91)</f>
+        <v>0.1</v>
       </c>
       <c r="I91" s="17" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="J91" s="20" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="K91" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L91" s="3" t="s">
-        <v>304</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L91" s="2"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="35">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B92" s="15">
-        <f>(5*G100)</f>
-        <v>10</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="D92" s="17" t="s">
-        <v>252</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>305</v>
+        <v>279</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="E92" s="21" t="s">
+        <v>259</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>306</v>
+        <v>260</v>
       </c>
       <c r="G92" s="19">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="H92" s="19">
-        <f>(B92*G92)</f>
-        <v>0.5</v>
+        <f t="shared" si="4"/>
+        <v>0.11</v>
       </c>
       <c r="I92" s="17" t="s">
         <v>81</v>
       </c>
       <c r="J92" s="20" t="s">
-        <v>208</v>
+        <v>168</v>
       </c>
       <c r="K92" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L92" s="2" t="s">
-        <v>307</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="L92" s="2"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="35">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B93" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="D93" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>263</v>
-      </c>
-      <c r="F93" s="21" t="s">
-        <v>264</v>
+        <f>(6*G98)</f>
+        <v>6</v>
+      </c>
+      <c r="C93" s="17"/>
+      <c r="D93" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E93" s="15">
+        <v>500588000</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>369</v>
       </c>
       <c r="G93" s="19">
         <v>0.1</v>
       </c>
       <c r="H93" s="19">
-        <f t="shared" ref="H93:H96" si="4">(B93*G93)</f>
-        <v>0.2</v>
-      </c>
-      <c r="I93" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="J93" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="K93" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L93" s="2"/>
+        <f t="shared" si="4"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I93" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="J93" s="20"/>
+      <c r="K93" s="17"/>
+      <c r="R93" s="2" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A94" s="35">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B94" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C94" s="17" t="s">
-        <v>291</v>
-      </c>
-      <c r="D94" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="E94" s="21" t="s">
-        <v>271</v>
-      </c>
-      <c r="F94" s="21" t="s">
-        <v>272</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C94" s="15"/>
+      <c r="D94" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E94" s="15" t="s">
+        <v>370</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>371</v>
       </c>
       <c r="G94" s="19">
-        <v>0.11</v>
+        <v>0.36</v>
       </c>
       <c r="H94" s="19">
         <f t="shared" si="4"/>
-        <v>0.22</v>
-      </c>
-      <c r="I94" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J94" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="K94" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="L94" s="2"/>
+        <v>0.36</v>
+      </c>
+      <c r="I94" s="27"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A95" s="35">
-        <v>23</v>
-      </c>
-      <c r="B95" s="15">
-        <f>(6*G100)</f>
-        <v>12</v>
-      </c>
-      <c r="C95" s="17"/>
-      <c r="D95" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E95" s="15">
-        <v>500588000</v>
-      </c>
-      <c r="F95" s="15" t="s">
-        <v>381</v>
-      </c>
-      <c r="G95" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="H95" s="19">
-        <f t="shared" si="4"/>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="I95" s="27" t="s">
-        <v>380</v>
-      </c>
-      <c r="J95" s="20"/>
-      <c r="K95" s="17"/>
-      <c r="R95" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A96" s="35">
-        <v>24</v>
-      </c>
-      <c r="B96" s="15">
-        <f>(1*G100)</f>
-        <v>2</v>
-      </c>
-      <c r="C96" s="15"/>
-      <c r="D96" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E96" s="15" t="s">
-        <v>382</v>
-      </c>
-      <c r="F96" s="15" t="s">
-        <v>383</v>
-      </c>
-      <c r="G96" s="19">
-        <v>0.36</v>
-      </c>
-      <c r="H96" s="19">
-        <f t="shared" si="4"/>
-        <v>0.72</v>
-      </c>
-      <c r="I96" s="27"/>
-      <c r="J96" s="15"/>
-      <c r="K96" s="15"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I99" s="12"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="F100" s="44" t="s">
-        <v>385</v>
-      </c>
-      <c r="G100" s="1">
-        <v>2</v>
-      </c>
-      <c r="H100" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="I100" s="5"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H101" s="9">
-        <f>SUM(H12:H71)</f>
-        <v>144.16</v>
-      </c>
-      <c r="I101" s="5"/>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H102" s="1"/>
-      <c r="I102" s="6"/>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H103" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I103" s="3"/>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H104" s="9">
-        <f>SUM(H75:H96)</f>
-        <v>32.299999999999997</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H106" s="7" t="s">
+      <c r="A95" s="1"/>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="I97" s="12"/>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F98" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="G98" s="1">
+        <v>1</v>
+      </c>
+      <c r="H98" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H99" s="9">
+        <f>SUM(H12:H69)</f>
+        <v>71.699999999999989</v>
+      </c>
+      <c r="I99" s="5"/>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H100" s="1"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H101" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H102" s="9">
+        <f>SUM(H73:H94)</f>
+        <v>16.149999999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H104" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H107" s="9">
-        <f>SUM(H101+H104)</f>
-        <v>176.45999999999998</v>
-      </c>
-    </row>
-    <row r="113" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H113" s="11"/>
+    <row r="105" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H105" s="9">
+        <f>SUM(H99+H102)</f>
+        <v>87.85</v>
+      </c>
+    </row>
+    <row r="111" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H111" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
small tweaks, BOM updated
</commit_message>
<xml_diff>
--- a/SPEX HAB2 BOM.xlsx
+++ b/SPEX HAB2 BOM.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Turnkey" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$54</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="383">
   <si>
     <t>Description</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Q4,Q5,Q6</t>
-  </si>
-  <si>
-    <t>Q101,Q104</t>
   </si>
   <si>
     <t>Q105</t>
@@ -1025,18 +1022,6 @@
   </si>
   <si>
     <t>SOT-23</t>
-  </si>
-  <si>
-    <t>DMG2302U-7</t>
-  </si>
-  <si>
-    <t>621-DMG2302U-7</t>
-  </si>
-  <si>
-    <t>Enable pin Nchannel Mosfet</t>
-  </si>
-  <si>
-    <t>SOT23-3</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Incorportated </t>
@@ -1883,10 +1868,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R111"/>
+  <dimension ref="A1:R110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I72" sqref="I72"/>
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1926,7 +1911,7 @@
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2013,7 +1998,7 @@
         <v>12</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2034,17 +2019,17 @@
         <v>1</v>
       </c>
       <c r="B12" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="F12" s="18"/>
       <c r="G12" s="19">
@@ -2055,16 +2040,16 @@
         <v>6.8</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J12" s="20" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L12" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
@@ -2072,20 +2057,20 @@
         <v>2</v>
       </c>
       <c r="B13" s="15">
-        <f>(3*G98)</f>
+        <f>(3*G97)</f>
         <v>3</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="18" t="s">
         <v>111</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>112</v>
       </c>
       <c r="G13" s="19">
         <v>0.55000000000000004</v>
@@ -2095,13 +2080,13 @@
         <v>1.6500000000000001</v>
       </c>
       <c r="I13" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
@@ -2109,20 +2094,20 @@
         <v>3</v>
       </c>
       <c r="B14" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E14" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="F14" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>114</v>
       </c>
       <c r="G14" s="19">
         <v>7.07</v>
@@ -2132,13 +2117,13 @@
         <v>7.07</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
@@ -2146,20 +2131,20 @@
         <v>4</v>
       </c>
       <c r="B15" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E15" s="22" t="s">
         <v>23</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="19">
         <v>0.48</v>
@@ -2169,13 +2154,13 @@
         <v>0.48</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J15" s="20" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2183,20 +2168,20 @@
         <v>5</v>
       </c>
       <c r="B16" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C16" s="25" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E16" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="17" t="s">
         <v>117</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>118</v>
       </c>
       <c r="G16" s="19">
         <v>1.22</v>
@@ -2206,13 +2191,13 @@
         <v>1.22</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J16" s="20" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2220,20 +2205,20 @@
         <v>6</v>
       </c>
       <c r="B17" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C17" s="25" t="s">
         <v>18</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G17" s="19">
         <v>5.66</v>
@@ -2243,13 +2228,13 @@
         <v>5.66</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2257,20 +2242,20 @@
         <v>7</v>
       </c>
       <c r="B18" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C18" s="25" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E18" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>121</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>122</v>
       </c>
       <c r="G18" s="26">
         <v>6.21</v>
@@ -2280,13 +2265,13 @@
         <v>6.21</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J18" s="20" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2294,20 +2279,20 @@
         <v>8</v>
       </c>
       <c r="B19" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>20</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="F19" s="27" t="s">
         <v>132</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>133</v>
       </c>
       <c r="G19" s="28">
         <v>2.12</v>
@@ -2317,13 +2302,13 @@
         <v>2.12</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J19" s="17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L19" s="2"/>
     </row>
@@ -2332,20 +2317,20 @@
         <v>10</v>
       </c>
       <c r="B20" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G20" s="19">
         <v>1.4</v>
@@ -2355,13 +2340,13 @@
         <v>1.4</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L20" s="2"/>
     </row>
@@ -2370,20 +2355,20 @@
         <v>11</v>
       </c>
       <c r="B21" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C21" s="24" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E21" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="15" t="s">
         <v>136</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>137</v>
       </c>
       <c r="G21" s="19">
         <v>0.8</v>
@@ -2393,11 +2378,11 @@
         <v>0.8</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J21" s="20"/>
       <c r="K21" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L21" s="2"/>
     </row>
@@ -2406,20 +2391,20 @@
         <v>12</v>
       </c>
       <c r="B22" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C22" s="25" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E22" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F22" s="29" t="s">
         <v>141</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>142</v>
       </c>
       <c r="G22" s="19">
         <v>4</v>
@@ -2429,13 +2414,13 @@
         <v>4</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J22" s="20" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2443,20 +2428,20 @@
         <v>13</v>
       </c>
       <c r="B23" s="15">
-        <f>(2*G98)</f>
+        <f>(2*G97)</f>
         <v>2</v>
       </c>
       <c r="C23" s="25" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E23" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="F23" s="15" t="s">
         <v>145</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>146</v>
       </c>
       <c r="G23" s="19">
         <v>1.45</v>
@@ -2466,13 +2451,13 @@
         <v>2.9</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J23" s="20" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2480,20 +2465,20 @@
         <v>14</v>
       </c>
       <c r="B24" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>28</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>149</v>
       </c>
       <c r="G24" s="28">
         <v>0.72</v>
@@ -2503,11 +2488,11 @@
         <v>0.72</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J24" s="20"/>
       <c r="K24" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -2515,20 +2500,20 @@
         <v>15</v>
       </c>
       <c r="B25" s="15">
-        <f>(2*G98)</f>
+        <f>(2*G97)</f>
         <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="D25" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E25" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="F25" s="29" t="s">
         <v>308</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>309</v>
       </c>
       <c r="G25" s="19">
         <v>0.42</v>
@@ -2538,13 +2523,13 @@
         <v>0.84</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="J25" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2552,20 +2537,20 @@
         <v>16</v>
       </c>
       <c r="B26" s="15">
-        <f>(3*G98)</f>
+        <f>(3*G97)</f>
         <v>3</v>
       </c>
       <c r="C26" s="25" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="25" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="F26" s="29" t="s">
         <v>304</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>305</v>
       </c>
       <c r="G26" s="19">
         <v>0.26</v>
@@ -2575,13 +2560,13 @@
         <v>0.78</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J26" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2589,20 +2574,20 @@
         <v>19</v>
       </c>
       <c r="B27" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E27" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>153</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="G27" s="19">
         <v>0.46</v>
@@ -2612,11 +2597,11 @@
         <v>0.46</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J27" s="20"/>
       <c r="K27" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2624,372 +2609,373 @@
         <v>20</v>
       </c>
       <c r="B28" s="15">
-        <f>(3*G98)</f>
+        <f>(3*G97)</f>
         <v>3</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>32</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E28" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="F28" s="15" t="s">
         <v>157</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>158</v>
       </c>
       <c r="G28" s="19">
         <v>0.52</v>
       </c>
       <c r="H28" s="19">
-        <f t="shared" ref="H28:H51" si="2">(B28*G28)</f>
+        <f t="shared" ref="H28:H50" si="2">(B28*G28)</f>
         <v>1.56</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J28" s="20"/>
       <c r="K28" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B29" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>33</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>327</v>
+        <v>161</v>
       </c>
       <c r="E29" s="15" t="s">
-        <v>323</v>
+        <v>159</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>324</v>
+        <v>160</v>
       </c>
       <c r="G29" s="19">
-        <v>0.37</v>
+        <v>0.52</v>
       </c>
       <c r="H29" s="19">
         <f t="shared" si="2"/>
-        <v>0.74</v>
+        <v>0.52</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="J29" s="20" t="s">
-        <v>326</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="J29" s="20"/>
       <c r="K29" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B30" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>34</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>162</v>
+        <v>110</v>
       </c>
       <c r="E30" s="15" t="s">
-        <v>160</v>
+        <v>317</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>161</v>
+        <v>318</v>
       </c>
       <c r="G30" s="19">
-        <v>0.52</v>
+        <v>0.1</v>
       </c>
       <c r="H30" s="19">
         <f t="shared" si="2"/>
-        <v>0.52</v>
+        <v>0.1</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="J30" s="20"/>
+        <v>320</v>
+      </c>
+      <c r="J30" s="20" t="s">
+        <v>321</v>
+      </c>
       <c r="K30" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="L30" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B31" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C31" s="25" t="s">
         <v>35</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>111</v>
+        <v>165</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>318</v>
+        <v>163</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>319</v>
+        <v>164</v>
       </c>
       <c r="G31" s="19">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="H31" s="19">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>321</v>
+        <v>166</v>
       </c>
       <c r="J31" s="20" t="s">
-        <v>322</v>
+        <v>167</v>
       </c>
       <c r="K31" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L31" t="s">
-        <v>320</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C32" s="25" t="s">
         <v>36</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>166</v>
+        <v>297</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>164</v>
+        <v>295</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>165</v>
+        <v>296</v>
       </c>
       <c r="G32" s="19">
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="H32" s="19">
         <f t="shared" si="2"/>
-        <v>0.13</v>
+        <v>0.15</v>
       </c>
       <c r="I32" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="J32" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="J32" s="20" t="s">
-        <v>168</v>
-      </c>
       <c r="K32" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L32" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B33" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C33" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="17" t="s">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="30" t="s">
         <v>298</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="F33" s="15" t="s">
+      <c r="D33" s="25" t="s">
         <v>297</v>
       </c>
+      <c r="E33" s="25" t="s">
+        <v>299</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>300</v>
+      </c>
       <c r="G33" s="19">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H33" s="19">
         <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="J33" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L33" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A34" s="33">
+        <v>28</v>
+      </c>
+      <c r="B34" s="15">
+        <f>(2*G97)</f>
+        <v>2</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="19">
         <v>0.15</v>
-      </c>
-      <c r="I33" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="J33" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="K33" s="17" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A34" s="14">
-        <v>26</v>
-      </c>
-      <c r="B34" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>299</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>298</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>300</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="G34" s="19">
-        <v>0.1</v>
       </c>
       <c r="H34" s="19">
         <f t="shared" si="2"/>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>302</v>
+        <v>171</v>
       </c>
       <c r="J34" s="20" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="K34" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L34" t="s">
-        <v>303</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L34" s="2"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A35" s="33">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B35" s="15">
-        <f>(2*G98)</f>
+        <f>(2*G97)</f>
         <v>2</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>38</v>
+      <c r="C35" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>171</v>
+        <v>322</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>328</v>
       </c>
       <c r="G35" s="19">
-        <v>0.15</v>
+        <v>0.19</v>
       </c>
       <c r="H35" s="19">
         <f t="shared" si="2"/>
-        <v>0.3</v>
-      </c>
-      <c r="I35" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="J35" s="20" t="s">
-        <v>173</v>
-      </c>
+        <v>0.38</v>
+      </c>
+      <c r="I35" s="17"/>
+      <c r="J35" s="20"/>
       <c r="K35" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L35" s="2"/>
+        <v>169</v>
+      </c>
+      <c r="L35" s="3"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A36" s="33">
-        <v>29</v>
+      <c r="A36" s="34">
+        <v>30</v>
       </c>
       <c r="B36" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
-      </c>
-      <c r="C36" s="15" t="s">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C36" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>332</v>
+        <v>110</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>330</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="G36" s="19">
-        <v>0.19</v>
+        <v>0</v>
       </c>
       <c r="H36" s="19">
         <f t="shared" si="2"/>
-        <v>0.38</v>
-      </c>
-      <c r="I36" s="17"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="15"/>
       <c r="J36" s="20"/>
       <c r="K36" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L36" s="3"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A37" s="34">
-        <v>30</v>
+      <c r="A37" s="33">
+        <v>31</v>
       </c>
       <c r="B37" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>41</v>
+        <v>323</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>111</v>
+        <v>333</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G37" s="19">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="H37" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I37" s="15"/>
+        <f>(B37*G37)</f>
+        <v>0.38</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>325</v>
+      </c>
       <c r="J37" s="20"/>
       <c r="K37" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L37" s="3"/>
       <c r="M37" s="1"/>
@@ -2997,115 +2983,117 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A38" s="33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B38" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E38" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="F38" s="13" t="s">
         <v>336</v>
       </c>
-      <c r="F38" s="13" t="s">
+      <c r="G38" s="19">
+        <v>0.48</v>
+      </c>
+      <c r="H38" s="19">
+        <f t="shared" si="2"/>
+        <v>0.48</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="J38" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="G38" s="19">
-        <v>0.38</v>
-      </c>
-      <c r="H38" s="19">
-        <f>(B38*G38)</f>
-        <v>0.38</v>
-      </c>
-      <c r="I38" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="J38" s="20"/>
       <c r="K38" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L38" s="3"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A39" s="33">
-        <v>32</v>
+      <c r="A39" s="34">
+        <v>33</v>
       </c>
       <c r="B39" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>329</v>
+        <v>41</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>340</v>
+        <v>322</v>
       </c>
       <c r="E39" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>341</v>
-      </c>
       <c r="G39" s="19">
-        <v>0.48</v>
+        <v>0.34</v>
       </c>
       <c r="H39" s="19">
         <f t="shared" si="2"/>
-        <v>0.48</v>
+        <v>0.34</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>331</v>
-      </c>
-      <c r="J39" s="20" t="s">
-        <v>342</v>
-      </c>
+        <v>340</v>
+      </c>
+      <c r="J39" s="20"/>
       <c r="K39" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L39" s="3"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A40" s="34">
-        <v>33</v>
+      <c r="A40" s="33">
+        <v>34</v>
       </c>
       <c r="B40" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>42</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>327</v>
+        <v>231</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>343</v>
+        <v>313</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>344</v>
+        <v>314</v>
       </c>
       <c r="G40" s="19">
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
       <c r="H40" s="19">
         <f t="shared" si="2"/>
-        <v>0.34</v>
+        <v>0.46</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>345</v>
-      </c>
-      <c r="J40" s="20"/>
+        <v>315</v>
+      </c>
+      <c r="J40" s="20" t="s">
+        <v>316</v>
+      </c>
       <c r="K40" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L40" s="3"/>
       <c r="M40" s="1"/>
@@ -3113,292 +3101,294 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A41" s="33">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C41" s="17" t="s">
+        <f>(2*G97)</f>
+        <v>2</v>
+      </c>
+      <c r="C41" s="27" t="s">
         <v>43</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="E41" s="15" t="s">
-        <v>314</v>
+        <v>192</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>315</v>
+        <v>174</v>
       </c>
       <c r="G41" s="19">
-        <v>0.46</v>
+        <v>1.43</v>
       </c>
       <c r="H41" s="19">
         <f t="shared" si="2"/>
-        <v>0.46</v>
+        <v>2.86</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="J41" s="20" t="s">
-        <v>317</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="J41" s="21"/>
       <c r="K41" s="17" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="L41" s="3"/>
       <c r="M41" s="1"/>
       <c r="N41" s="1"/>
+      <c r="R41" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A42" s="33">
-        <v>35</v>
+      <c r="A42" s="34">
+        <v>36</v>
       </c>
       <c r="B42" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>194</v>
+        <v>344</v>
       </c>
       <c r="E42" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="F42" s="15" t="s">
-        <v>175</v>
+        <v>341</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>342</v>
       </c>
       <c r="G42" s="19">
-        <v>1.43</v>
+        <v>0.97</v>
       </c>
       <c r="H42" s="19">
         <f t="shared" si="2"/>
-        <v>2.86</v>
+        <v>0.97</v>
       </c>
       <c r="I42" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="J42" s="20"/>
+      <c r="K42" s="17" t="s">
         <v>176</v>
-      </c>
-      <c r="J42" s="21"/>
-      <c r="K42" s="17" t="s">
-        <v>177</v>
       </c>
       <c r="L42" s="3"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
-      <c r="R42" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A43" s="34">
-        <v>36</v>
+    </row>
+    <row r="43" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="33">
+        <v>37</v>
       </c>
       <c r="B43" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C43" s="27" t="s">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D43" s="17" t="s">
-        <v>349</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F43" s="17" t="s">
-        <v>347</v>
-      </c>
-      <c r="G43" s="19">
-        <v>0.97</v>
-      </c>
+      <c r="D43" s="17"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="19"/>
       <c r="H43" s="19">
         <f t="shared" si="2"/>
-        <v>0.97</v>
-      </c>
-      <c r="I43" s="17" t="s">
-        <v>348</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I43" s="17"/>
       <c r="J43" s="20"/>
-      <c r="K43" s="17" t="s">
-        <v>177</v>
-      </c>
+      <c r="K43" s="17"/>
       <c r="L43" s="3"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:18" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A44" s="33">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B44" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C44" s="17" t="s">
+        <f>(4*G97)</f>
+        <v>4</v>
+      </c>
+      <c r="C44" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="19"/>
+      <c r="D44" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" s="17"/>
+      <c r="F44" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="G44" s="19">
+        <v>1.5</v>
+      </c>
       <c r="H44" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="17"/>
-      <c r="L44" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="I44" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="J44" s="36" t="s">
+        <v>270</v>
+      </c>
+      <c r="K44" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>180</v>
+      </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A45" s="33">
-        <v>38</v>
+      <c r="A45" s="34">
+        <v>39</v>
       </c>
       <c r="B45" s="15">
-        <f>(4*G98)</f>
-        <v>4</v>
+        <f>(7*G97)</f>
+        <v>7</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" s="17"/>
+        <v>90</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>177</v>
+      </c>
       <c r="F45" s="15" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G45" s="19">
-        <v>1.5</v>
+        <v>0.72</v>
       </c>
       <c r="H45" s="19">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="I45" s="32" t="s">
-        <v>183</v>
-      </c>
-      <c r="J45" s="36" t="s">
-        <v>271</v>
+        <v>5.04</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="J45" s="17" t="s">
+        <v>270</v>
       </c>
       <c r="K45" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>181</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="L45" s="3"/>
       <c r="M45" s="1"/>
       <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A46" s="34">
-        <v>39</v>
+      <c r="A46" s="33">
+        <v>40</v>
       </c>
       <c r="B46" s="15">
-        <f>(7*G98)</f>
-        <v>7</v>
-      </c>
-      <c r="C46" s="27" t="s">
+        <f>(4*G97)</f>
+        <v>4</v>
+      </c>
+      <c r="C46" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="D46" s="27" t="s">
-        <v>91</v>
+      <c r="D46" s="17" t="s">
+        <v>199</v>
       </c>
       <c r="E46" s="15" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>179</v>
+        <v>197</v>
       </c>
       <c r="G46" s="19">
-        <v>0.72</v>
+        <v>0.1</v>
       </c>
       <c r="H46" s="19">
         <f t="shared" si="2"/>
-        <v>5.04</v>
+        <v>0.4</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>271</v>
+        <v>49</v>
+      </c>
+      <c r="J46" s="20" t="s">
+        <v>167</v>
       </c>
       <c r="K46" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="L46" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>201</v>
+      </c>
       <c r="M46" s="1"/>
       <c r="N46" s="1"/>
+      <c r="R46" s="2" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A47" s="33">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B47" s="15">
-        <f>(4*G98)</f>
-        <v>4</v>
+        <f>(18*G97)</f>
+        <v>18</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>49</v>
+        <v>377</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>199</v>
-      </c>
-      <c r="F47" s="15" t="s">
-        <v>198</v>
+        <v>202</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>203</v>
       </c>
       <c r="G47" s="19">
         <v>0.1</v>
       </c>
       <c r="H47" s="19">
         <f t="shared" si="2"/>
-        <v>0.4</v>
+        <v>1.8</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J47" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K47" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L47" s="3" t="s">
-        <v>202</v>
+        <v>169</v>
       </c>
       <c r="M47" s="1"/>
       <c r="N47" s="1"/>
       <c r="R47" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="33">
-        <v>41</v>
+      <c r="A48" s="34">
+        <v>42</v>
       </c>
       <c r="B48" s="15">
-        <f>(18*G98)</f>
-        <v>18</v>
-      </c>
-      <c r="C48" s="17" t="s">
-        <v>382</v>
+        <f>(2*G97)</f>
+        <v>2</v>
+      </c>
+      <c r="C48" s="27" t="s">
+        <v>50</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="F48" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="F48" s="15" t="s">
         <v>204</v>
       </c>
       <c r="G48" s="19">
@@ -3406,285 +3396,283 @@
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J48" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K48" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
-      <c r="R48" s="2" t="s">
-        <v>201</v>
-      </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="34">
-        <v>42</v>
+      <c r="A49" s="33">
+        <v>43</v>
       </c>
       <c r="B49" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(3*G97)</f>
+        <v>3</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D49" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E49" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="F49" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="E49" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="F49" s="15" t="s">
-        <v>205</v>
       </c>
       <c r="G49" s="19">
         <v>0.1</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
       <c r="J49" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K49" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
+      </c>
+      <c r="L49" t="s">
+        <v>211</v>
       </c>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="33">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B50" s="15">
-        <f>(3*G98)</f>
-        <v>3</v>
-      </c>
-      <c r="C50" s="27" t="s">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C50" s="17" t="s">
         <v>54</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="G50" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>0.30000000000000004</v>
+        <v>0.08</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>211</v>
+        <v>55</v>
       </c>
       <c r="J50" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K50" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L50" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="33">
-        <v>44</v>
+      <c r="A51" s="34">
+        <v>45</v>
       </c>
       <c r="B51" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(5*G97)</f>
+        <v>5</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F51" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="G51" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H51" s="19">
+        <f t="shared" ref="H51:H88" si="3">(B51*G51)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I51" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J51" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K51" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="R51" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="33">
+        <v>46</v>
+      </c>
+      <c r="B52" s="15">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>376</v>
+      </c>
+      <c r="D52" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G51" s="19">
+      <c r="E52" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="G52" s="19">
         <v>0.08</v>
       </c>
-      <c r="H51" s="19">
-        <f t="shared" si="2"/>
+      <c r="H52" s="19">
+        <f t="shared" si="3"/>
         <v>0.08</v>
-      </c>
-      <c r="I51" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J51" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="K51" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L51" t="s">
-        <v>217</v>
-      </c>
-      <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="34">
-        <v>45</v>
-      </c>
-      <c r="B52" s="15">
-        <f>(5*G98)</f>
-        <v>5</v>
-      </c>
-      <c r="C52" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D52" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="E52" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="F52" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="G52" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="H52" s="19">
-        <f t="shared" ref="H52:H89" si="3">(B52*G52)</f>
-        <v>0.5</v>
       </c>
       <c r="I52" s="17" t="s">
         <v>58</v>
       </c>
       <c r="J52" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K52" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L52" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="R52" s="2" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A53" s="33">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B53" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(2*G97)</f>
+        <v>2</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>381</v>
+        <v>60</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G53" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H53" s="19">
         <f t="shared" si="3"/>
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="I53" s="17" t="s">
         <v>59</v>
       </c>
       <c r="J53" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K53" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L53" s="3" t="s">
-        <v>217</v>
+        <v>169</v>
+      </c>
+      <c r="L53" s="31" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="33">
-        <v>47</v>
+      <c r="A54" s="34">
+        <v>48</v>
       </c>
       <c r="B54" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>61</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="E54" s="17" t="s">
-        <v>223</v>
+        <v>199</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>225</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G54" s="19">
         <v>0.1</v>
       </c>
       <c r="H54" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I54" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J54" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K54" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L54" s="31" t="s">
-        <v>225</v>
+        <v>169</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="34">
-        <v>48</v>
+      <c r="A55" s="33">
+        <v>49</v>
       </c>
       <c r="B55" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(2*G97)</f>
+        <v>2</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>227</v>
@@ -3694,80 +3682,80 @@
       </c>
       <c r="H55" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I55" s="17" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="J55" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K55" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A56" s="33">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B56" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C56" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="E56" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E56" s="25" t="s">
         <v>229</v>
       </c>
-      <c r="F56" s="15" t="s">
-        <v>228</v>
+      <c r="F56" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="G56" s="19">
         <v>0.1</v>
       </c>
       <c r="H56" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I56" s="17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="J56" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K56" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L56" s="3" t="s">
-        <v>202</v>
+        <v>169</v>
+      </c>
+      <c r="L56" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="33">
-        <v>50</v>
+      <c r="A57" s="34">
+        <v>51</v>
       </c>
       <c r="B57" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="E57" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="F57" s="17" t="s">
-        <v>231</v>
+        <v>67</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="F57" s="15" t="s">
+        <v>234</v>
       </c>
       <c r="G57" s="19">
         <v>0.1</v>
@@ -3777,391 +3765,389 @@
         <v>0.1</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="J57" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K57" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L57" t="s">
-        <v>233</v>
+        <v>169</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="34">
-        <v>51</v>
+      <c r="A58" s="33">
+        <v>52</v>
       </c>
       <c r="B58" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="G58" s="19">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="H58" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J58" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K58" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>202</v>
+        <v>238</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="33">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B59" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(8*G97)</f>
+        <v>8</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>237</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="F59" s="15" t="s">
-        <v>238</v>
+        <v>71</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E59" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="F59" s="21" t="s">
+        <v>243</v>
       </c>
       <c r="G59" s="19">
-        <v>0.09</v>
+        <v>0.08</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="3"/>
-        <v>0.09</v>
+        <v>0.64</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J59" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K59" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L59" s="3" t="s">
-        <v>239</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L59" s="3"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="33">
-        <v>53</v>
+      <c r="A60" s="34">
+        <v>54</v>
       </c>
       <c r="B60" s="15">
-        <f>(8*G98)</f>
-        <v>8</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>72</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>243</v>
+        <v>252</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>250</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="G60" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="3"/>
-        <v>0.64</v>
+        <v>0.1</v>
       </c>
       <c r="I60" s="17" t="s">
         <v>74</v>
       </c>
       <c r="J60" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L60" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="34">
-        <v>54</v>
+      <c r="A61" s="33">
+        <v>55</v>
       </c>
       <c r="B61" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(8*G97)</f>
+        <v>8</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>73</v>
+        <v>248</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>251</v>
+        <v>239</v>
+      </c>
+      <c r="E61" s="21" t="s">
+        <v>241</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G61" s="19">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.32</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="J61" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K61" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L61" s="3" t="s">
-        <v>254</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L61" s="3"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="33">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B62" s="15">
-        <f>(8*G98)</f>
-        <v>8</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>249</v>
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>244</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G62" s="19">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="3"/>
-        <v>0.32</v>
+        <v>0.02</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>250</v>
+        <v>75</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
       <c r="K62" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L62" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="33">
-        <v>56</v>
+      <c r="A63" s="34">
+        <v>57</v>
       </c>
       <c r="B63" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C63" s="32" t="s">
-        <v>245</v>
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>76</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="G63" s="19">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="3"/>
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="I63" s="17" t="s">
-        <v>76</v>
+        <v>254</v>
       </c>
       <c r="J63" s="20" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="K63" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L63" s="3" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="34">
-        <v>57</v>
+      <c r="A64" s="33">
+        <v>58</v>
       </c>
       <c r="B64" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>77</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="F64" s="21" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="G64" s="19">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="3"/>
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>255</v>
+        <v>80</v>
       </c>
       <c r="J64" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K64" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L64" s="3" t="s">
-        <v>258</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L64" s="3"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="33">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B65" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(2*G97)</f>
+        <v>2</v>
       </c>
       <c r="C65" s="17" t="s">
         <v>78</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>259</v>
+        <v>369</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>260</v>
+        <v>370</v>
       </c>
       <c r="G65" s="19">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="3"/>
-        <v>0.11</v>
+        <v>0.4</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J65" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K65" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L65" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="33">
-        <v>59</v>
+      <c r="A66" s="34">
+        <v>60</v>
       </c>
       <c r="B66" s="15">
-        <f>(2*G98)</f>
+        <f>(2*G97)</f>
         <v>2</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="D66" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E66" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="21" t="s">
-        <v>374</v>
-      </c>
       <c r="F66" s="21" t="s">
-        <v>375</v>
+        <v>263</v>
       </c>
       <c r="G66" s="19">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>168</v>
+        <v>194</v>
       </c>
       <c r="K66" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L66" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="L66" s="3"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A67" s="33">
+        <v>61</v>
+      </c>
+      <c r="B67" s="15">
+        <f>(2*G97)</f>
+        <v>2</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="20" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="34">
-        <v>60</v>
-      </c>
-      <c r="B67" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
-      </c>
-      <c r="C67" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="D67" s="20" t="s">
-        <v>253</v>
-      </c>
       <c r="E67" s="21" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G67" s="19">
         <v>0.5</v>
@@ -4171,553 +4157,553 @@
         <v>1</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J67" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K67" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L67" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L67" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="33">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B68" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(3*G97)</f>
+        <v>3</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="G68" s="19">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I68" s="17" t="s">
         <v>84</v>
       </c>
       <c r="J68" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="K68" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="33">
-        <v>62</v>
+      <c r="A69" s="34">
+        <v>63</v>
       </c>
       <c r="B69" s="15">
-        <f>(3*G98)</f>
-        <v>3</v>
-      </c>
-      <c r="C69" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="D69" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="E69" s="21" t="s">
-        <v>267</v>
-      </c>
-      <c r="F69" s="21" t="s">
-        <v>268</v>
+        <f>(7*G97)</f>
+        <v>7</v>
+      </c>
+      <c r="C69" s="17"/>
+      <c r="D69" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F69" s="15" t="s">
+        <v>183</v>
       </c>
       <c r="G69" s="19">
-        <v>0.1</v>
+        <v>0.31</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>2.17</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="J69" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="K69" s="17" t="s">
-        <v>170</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="J69" s="20"/>
+      <c r="K69" s="17"/>
       <c r="L69" s="3" t="s">
-        <v>270</v>
+        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="34">
-        <v>63</v>
+      <c r="A70" s="33">
+        <v>64</v>
       </c>
       <c r="B70" s="15">
-        <f>(7*G98)</f>
-        <v>7</v>
+        <f>(14*G97)</f>
+        <v>14</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E70" s="15" t="s">
-        <v>185</v>
+        <v>90</v>
+      </c>
+      <c r="E70" s="15">
+        <v>1722533123</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="G70" s="19">
-        <v>0.31</v>
+        <v>0.152</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" si="3"/>
-        <v>2.17</v>
+        <v>2.1280000000000001</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J70" s="20"/>
       <c r="K70" s="17"/>
       <c r="L70" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
+      </c>
+      <c r="R70" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="33">
-        <v>64</v>
-      </c>
-      <c r="B71" s="15">
-        <f>(14*G98)</f>
-        <v>14</v>
-      </c>
-      <c r="C71" s="17"/>
-      <c r="D71" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="15">
-        <v>1722533123</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="G71" s="19">
-        <v>0.152</v>
-      </c>
-      <c r="H71" s="19">
+      <c r="A71" s="37"/>
+      <c r="B71" s="37"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="39"/>
+      <c r="H71" s="39"/>
+      <c r="I71" s="38"/>
+      <c r="J71" s="40"/>
+      <c r="K71" s="37"/>
+      <c r="L71" s="3"/>
+    </row>
+    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A72" s="35">
+        <v>1</v>
+      </c>
+      <c r="B72" s="15">
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="E72" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="G72" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="H72" s="19">
         <f t="shared" si="3"/>
-        <v>2.1280000000000001</v>
-      </c>
-      <c r="I71" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="J71" s="20"/>
-      <c r="K71" s="17"/>
-      <c r="L71" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="R71" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="37"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="38"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="37"/>
-      <c r="G72" s="39"/>
-      <c r="H72" s="39"/>
-      <c r="I72" s="38"/>
-      <c r="J72" s="40"/>
-      <c r="K72" s="37"/>
+        <v>1.4</v>
+      </c>
+      <c r="I72" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J72" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="K72" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B73" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C73" s="17" t="s">
-        <v>15</v>
+        <v>92</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>124</v>
+        <v>357</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>25</v>
+        <v>353</v>
       </c>
       <c r="F73" s="15" t="s">
-        <v>135</v>
+        <v>354</v>
       </c>
       <c r="G73" s="19">
-        <v>1.4</v>
+        <v>0.64</v>
       </c>
       <c r="H73" s="19">
         <f t="shared" si="3"/>
-        <v>1.4</v>
+        <v>0.64</v>
       </c>
       <c r="I73" s="17" t="s">
-        <v>140</v>
+        <v>355</v>
       </c>
       <c r="J73" s="20" t="s">
-        <v>272</v>
+        <v>356</v>
       </c>
       <c r="K73" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A74" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B74" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C74" s="17" t="s">
-        <v>93</v>
+        <v>14</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>362</v>
+        <v>114</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F74" s="15" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="G74" s="19">
-        <v>0.64</v>
+        <v>1.24</v>
       </c>
       <c r="H74" s="19">
         <f t="shared" si="3"/>
-        <v>0.64</v>
+        <v>1.24</v>
       </c>
       <c r="I74" s="17" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="J74" s="20" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="K74" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L74" s="3"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A75" s="35">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B75" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C75" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D75" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E75" s="17" t="s">
-        <v>354</v>
-      </c>
-      <c r="F75" s="15" t="s">
-        <v>355</v>
+        <v>93</v>
+      </c>
+      <c r="D75" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F75" s="17" t="s">
+        <v>119</v>
       </c>
       <c r="G75" s="19">
-        <v>1.24</v>
+        <v>5.66</v>
       </c>
       <c r="H75" s="19">
-        <f t="shared" si="3"/>
-        <v>1.24</v>
+        <f>(B75*G75)</f>
+        <v>5.66</v>
       </c>
       <c r="I75" s="17" t="s">
-        <v>356</v>
+        <v>129</v>
       </c>
       <c r="J75" s="20" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="K75" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L75" s="3"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B76" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C76" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D76" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="E76" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F76" s="17" t="s">
-        <v>120</v>
+        <v>17</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="F76" s="15" t="s">
+        <v>372</v>
       </c>
       <c r="G76" s="19">
-        <v>5.66</v>
+        <v>2.84</v>
       </c>
       <c r="H76" s="19">
-        <f>(B76*G76)</f>
-        <v>5.66</v>
+        <f t="shared" si="3"/>
+        <v>2.84</v>
       </c>
       <c r="I76" s="17" t="s">
-        <v>130</v>
+        <v>272</v>
       </c>
       <c r="J76" s="20" t="s">
-        <v>350</v>
+        <v>273</v>
       </c>
       <c r="K76" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L76" s="3"/>
+      <c r="R76" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A77" s="35">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B77" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C77" s="17" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
       <c r="D77" s="17" t="s">
         <v>312</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>376</v>
+        <v>95</v>
       </c>
       <c r="F77" s="15" t="s">
-        <v>377</v>
+        <v>274</v>
       </c>
       <c r="G77" s="19">
-        <v>2.84</v>
+        <v>0.86</v>
       </c>
       <c r="H77" s="19">
         <f t="shared" si="3"/>
-        <v>2.84</v>
+        <v>0.86</v>
       </c>
       <c r="I77" s="17" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="J77" s="20" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="K77" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L77" s="3"/>
-      <c r="R77" s="2" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="35">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B78" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C78" s="17" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="E78" s="17" t="s">
-        <v>96</v>
+        <v>297</v>
+      </c>
+      <c r="E78" s="15" t="s">
+        <v>295</v>
       </c>
       <c r="F78" s="15" t="s">
-        <v>275</v>
+        <v>296</v>
       </c>
       <c r="G78" s="19">
-        <v>0.86</v>
+        <v>0.15</v>
       </c>
       <c r="H78" s="19">
         <f t="shared" si="3"/>
-        <v>0.86</v>
+        <v>0.15</v>
       </c>
       <c r="I78" s="17" t="s">
-        <v>276</v>
+        <v>217</v>
       </c>
       <c r="J78" s="20" t="s">
-        <v>277</v>
+        <v>167</v>
       </c>
       <c r="K78" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L78" s="3"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="35">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B79" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="E79" s="15" t="s">
-        <v>296</v>
+        <v>90</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>97</v>
       </c>
       <c r="F79" s="15" t="s">
-        <v>297</v>
+        <v>277</v>
       </c>
       <c r="G79" s="19">
-        <v>0.15</v>
+        <v>0.67</v>
       </c>
       <c r="H79" s="19">
         <f t="shared" si="3"/>
-        <v>0.15</v>
+        <v>0.67</v>
       </c>
       <c r="I79" s="17" t="s">
-        <v>218</v>
+        <v>96</v>
       </c>
       <c r="J79" s="20" t="s">
-        <v>168</v>
+        <v>270</v>
       </c>
       <c r="K79" s="17" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="L79" s="3"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="35">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B80" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D80" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E80" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="F80" s="15" t="s">
-        <v>278</v>
-      </c>
-      <c r="G80" s="19">
-        <v>0.67</v>
-      </c>
+      <c r="D80" s="17"/>
+      <c r="E80" s="15"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="19"/>
       <c r="H80" s="19">
         <f t="shared" si="3"/>
-        <v>0.67</v>
-      </c>
-      <c r="I80" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="J80" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="K80" s="17" t="s">
-        <v>177</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I80" s="17"/>
+      <c r="J80" s="20"/>
+      <c r="K80" s="15"/>
       <c r="L80" s="3"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="35">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B81" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="D81" s="17"/>
-      <c r="E81" s="15"/>
       <c r="F81" s="15"/>
       <c r="G81" s="19"/>
       <c r="H81" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I81" s="17"/>
       <c r="J81" s="20"/>
       <c r="K81" s="15"/>
       <c r="L81" s="3"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="35">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B82" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D82" s="17"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="19"/>
+        <v>98</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E82" s="15" t="s">
+        <v>287</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="G82" s="19">
+        <v>0.1</v>
+      </c>
       <c r="H82" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J82" s="20"/>
-      <c r="K82" s="15"/>
+        <v>0.1</v>
+      </c>
+      <c r="I82" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="J82" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="K82" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="L82" s="3"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="35">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B83" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="G83" s="19">
         <v>0.1</v>
@@ -4727,32 +4713,32 @@
         <v>0.1</v>
       </c>
       <c r="I83" s="17" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J83" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K83" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L83" s="3"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="35">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B84" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(3*G97)</f>
+        <v>3</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>101</v>
+        <v>347</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F84" s="15" t="s">
         <v>283</v>
@@ -4762,450 +4748,412 @@
       </c>
       <c r="H84" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I84" s="17" t="s">
         <v>102</v>
       </c>
       <c r="J84" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K84" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L84" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L84" s="3" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="35">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B85" s="15">
-        <f>(3*G98)</f>
-        <v>3</v>
+        <f>(2*G97)</f>
+        <v>2</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>352</v>
+        <v>103</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E85" s="15" t="s">
         <v>285</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G85" s="19">
         <v>0.1</v>
       </c>
       <c r="H85" s="19">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="I85" s="17" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="J85" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K85" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="35">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B86" s="15">
-        <f>(2*G98)</f>
-        <v>2</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C86" s="17" t="s">
         <v>104</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="G86" s="19">
         <v>0.1</v>
       </c>
       <c r="H86" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="I86" s="17" t="s">
         <v>58</v>
       </c>
       <c r="J86" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K86" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>202</v>
+        <v>291</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="35">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B87" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>105</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>290</v>
-      </c>
-      <c r="F87" s="15" t="s">
-        <v>291</v>
+        <v>360</v>
+      </c>
+      <c r="E87" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="F87" s="21" t="s">
+        <v>358</v>
       </c>
       <c r="G87" s="19">
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="I87" s="17" t="s">
-        <v>59</v>
+        <v>348</v>
       </c>
       <c r="J87" s="20" t="s">
-        <v>196</v>
+        <v>280</v>
       </c>
       <c r="K87" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L87" s="3" t="s">
-        <v>292</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L87" s="3"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="35">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B88" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>106</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>365</v>
+        <v>214</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G88" s="19">
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="H88" s="19">
         <f t="shared" si="3"/>
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="I88" s="17" t="s">
-        <v>353</v>
+        <v>49</v>
       </c>
       <c r="J88" s="20" t="s">
-        <v>281</v>
+        <v>195</v>
       </c>
       <c r="K88" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L88" s="3"/>
+        <v>169</v>
+      </c>
+      <c r="L88" s="3" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="35">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B89" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
+        <f>(5*G97)</f>
+        <v>5</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>107</v>
+        <v>367</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>215</v>
-      </c>
-      <c r="E89" s="21" t="s">
-        <v>366</v>
+        <v>239</v>
+      </c>
+      <c r="E89" s="20" t="s">
+        <v>292</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>367</v>
+        <v>293</v>
       </c>
       <c r="G89" s="19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H89" s="19">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
+        <f>(B89*G89)</f>
+        <v>0.25</v>
       </c>
       <c r="I89" s="17" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="J89" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="K89" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L89" s="3" t="s">
-        <v>292</v>
+        <v>169</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="35">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B90" s="15">
-        <f>(5*G98)</f>
-        <v>5</v>
+        <f>(1*G97)</f>
+        <v>1</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>372</v>
-      </c>
-      <c r="D90" s="17" t="s">
-        <v>240</v>
+        <v>279</v>
+      </c>
+      <c r="D90" s="20" t="s">
+        <v>252</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="G90" s="19">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H90" s="19">
-        <f>(B90*G90)</f>
-        <v>0.25</v>
+        <f t="shared" ref="H90:H93" si="4">(B90*G90)</f>
+        <v>0.1</v>
       </c>
       <c r="I90" s="17" t="s">
         <v>74</v>
       </c>
       <c r="J90" s="20" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="K90" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L90" s="2" t="s">
-        <v>295</v>
-      </c>
+        <v>169</v>
+      </c>
+      <c r="L90" s="2"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="35">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B91" s="15">
-        <f>(1*G98)</f>
+        <f>(1*G97)</f>
         <v>1</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D91" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E91" s="20" t="s">
-        <v>251</v>
+        <v>252</v>
+      </c>
+      <c r="E91" s="21" t="s">
+        <v>258</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="G91" s="19">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="H91" s="19">
-        <f t="shared" ref="H91:H94" si="4">(B91*G91)</f>
-        <v>0.1</v>
+        <f t="shared" si="4"/>
+        <v>0.11</v>
       </c>
       <c r="I91" s="17" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="J91" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K91" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="L91" s="2"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A92" s="35">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B92" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D92" s="20" t="s">
-        <v>253</v>
-      </c>
-      <c r="E92" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="F92" s="21" t="s">
-        <v>260</v>
+        <f>(6*G97)</f>
+        <v>6</v>
+      </c>
+      <c r="C92" s="17"/>
+      <c r="D92" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E92" s="15">
+        <v>500588000</v>
+      </c>
+      <c r="F92" s="15" t="s">
+        <v>364</v>
       </c>
       <c r="G92" s="19">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="H92" s="19">
         <f t="shared" si="4"/>
-        <v>0.11</v>
-      </c>
-      <c r="I92" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="J92" s="20" t="s">
-        <v>168</v>
-      </c>
-      <c r="K92" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="L92" s="2"/>
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="I92" s="27" t="s">
+        <v>363</v>
+      </c>
+      <c r="J92" s="20"/>
+      <c r="K92" s="17"/>
+      <c r="R92" s="2" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A93" s="35">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B93" s="15">
-        <f>(6*G98)</f>
-        <v>6</v>
-      </c>
-      <c r="C93" s="17"/>
+        <f>(1*G97)</f>
+        <v>1</v>
+      </c>
+      <c r="C93" s="15"/>
       <c r="D93" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E93" s="15">
-        <v>500588000</v>
+        <v>90</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>365</v>
       </c>
       <c r="F93" s="15" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="G93" s="19">
-        <v>0.1</v>
+        <v>0.36</v>
       </c>
       <c r="H93" s="19">
         <f t="shared" si="4"/>
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="I93" s="27" t="s">
+        <v>0.36</v>
+      </c>
+      <c r="I93" s="27"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="15"/>
+    </row>
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+    </row>
+    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="I96" s="12"/>
+    </row>
+    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F97" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="J93" s="20"/>
-      <c r="K93" s="17"/>
-      <c r="R93" s="2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="35">
-        <v>24</v>
-      </c>
-      <c r="B94" s="15">
-        <f>(1*G98)</f>
-        <v>1</v>
-      </c>
-      <c r="C94" s="15"/>
-      <c r="D94" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="E94" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="F94" s="15" t="s">
-        <v>371</v>
-      </c>
-      <c r="G94" s="19">
-        <v>0.36</v>
-      </c>
-      <c r="H94" s="19">
-        <f t="shared" si="4"/>
-        <v>0.36</v>
-      </c>
-      <c r="I94" s="27"/>
-      <c r="J94" s="15"/>
-      <c r="K94" s="15"/>
-    </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A95" s="1"/>
-    </row>
-    <row r="97" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="I97" s="12"/>
+      <c r="G97" s="1">
+        <v>1</v>
+      </c>
+      <c r="H97" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I97" s="5"/>
     </row>
     <row r="98" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F98" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="G98" s="1">
-        <v>1</v>
-      </c>
-      <c r="H98" s="10" t="s">
+      <c r="H98" s="9">
+        <f>SUM(H12:H70)</f>
+        <v>75.257999999999996</v>
+      </c>
+      <c r="I98" s="5"/>
+    </row>
+    <row r="99" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H99" s="1"/>
+      <c r="I99" s="6"/>
+    </row>
+    <row r="100" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H100" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I98" s="5"/>
-    </row>
-    <row r="99" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H99" s="9">
-        <f>SUM(H12:H69)</f>
-        <v>71.699999999999989</v>
-      </c>
-      <c r="I99" s="5"/>
-    </row>
-    <row r="100" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H100" s="1"/>
-      <c r="I100" s="6"/>
+      <c r="I100" s="3"/>
     </row>
     <row r="101" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H101" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I101" s="3"/>
-    </row>
-    <row r="102" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H102" s="9">
-        <f>SUM(H73:H94)</f>
+      <c r="H101" s="9">
+        <f>SUM(H72:H93)</f>
         <v>16.149999999999999</v>
       </c>
     </row>
+    <row r="103" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H103" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
     <row r="104" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H104" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="105" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H105" s="9">
-        <f>SUM(H99+H102)</f>
-        <v>87.85</v>
-      </c>
-    </row>
-    <row r="111" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H111" s="11"/>
+      <c r="H104" s="9">
+        <f>SUM(H98+H101)</f>
+        <v>91.407999999999987</v>
+      </c>
+    </row>
+    <row r="110" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H110" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Continued tweaks, updated BOM again
</commit_message>
<xml_diff>
--- a/SPEX HAB2 BOM.xlsx
+++ b/SPEX HAB2 BOM.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Turnkey" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Turnkey!$A$1:$K$55</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="387">
   <si>
     <t>Description</t>
   </si>
@@ -1205,6 +1205,18 @@
   </si>
   <si>
     <t>SOT-23-6</t>
+  </si>
+  <si>
+    <t>R21,R22</t>
+  </si>
+  <si>
+    <t>51k ohm resistor</t>
+  </si>
+  <si>
+    <t>RK73B1JTTDD513J</t>
+  </si>
+  <si>
+    <t>660-RK73B1JTTDD513J</t>
   </si>
 </sst>
 </file>
@@ -1868,10 +1880,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R110"/>
+  <dimension ref="A1:R111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2019,7 +2031,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C12" s="17" t="s">
@@ -2057,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="15">
-        <f>(3*G97)</f>
+        <f>(3*G98)</f>
         <v>3</v>
       </c>
       <c r="C13" s="17" t="s">
@@ -2094,7 +2106,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C14" s="17" t="s">
@@ -2131,7 +2143,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C15" s="25" t="s">
@@ -2168,7 +2180,7 @@
         <v>5</v>
       </c>
       <c r="B16" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -2205,7 +2217,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -2242,7 +2254,7 @@
         <v>7</v>
       </c>
       <c r="B18" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C18" s="25" t="s">
@@ -2279,7 +2291,7 @@
         <v>8</v>
       </c>
       <c r="B19" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C19" s="30" t="s">
@@ -2317,7 +2329,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C20" s="17" t="s">
@@ -2355,7 +2367,7 @@
         <v>11</v>
       </c>
       <c r="B21" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C21" s="24" t="s">
@@ -2391,7 +2403,7 @@
         <v>12</v>
       </c>
       <c r="B22" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C22" s="25" t="s">
@@ -2428,7 +2440,7 @@
         <v>13</v>
       </c>
       <c r="B23" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C23" s="25" t="s">
@@ -2465,7 +2477,7 @@
         <v>14</v>
       </c>
       <c r="B24" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C24" s="30" t="s">
@@ -2500,7 +2512,7 @@
         <v>15</v>
       </c>
       <c r="B25" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C25" s="25" t="s">
@@ -2537,7 +2549,7 @@
         <v>16</v>
       </c>
       <c r="B26" s="15">
-        <f>(3*G97)</f>
+        <f>(3*G98)</f>
         <v>3</v>
       </c>
       <c r="C26" s="25" t="s">
@@ -2574,7 +2586,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C27" s="25" t="s">
@@ -2609,7 +2621,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="15">
-        <f>(3*G97)</f>
+        <f>(3*G98)</f>
         <v>3</v>
       </c>
       <c r="C28" s="25" t="s">
@@ -2628,7 +2640,7 @@
         <v>0.52</v>
       </c>
       <c r="H28" s="19">
-        <f t="shared" ref="H28:H50" si="2">(B28*G28)</f>
+        <f t="shared" ref="H28:H51" si="2">(B28*G28)</f>
         <v>1.56</v>
       </c>
       <c r="I28" s="17" t="s">
@@ -2644,7 +2656,7 @@
         <v>22</v>
       </c>
       <c r="B29" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C29" s="25" t="s">
@@ -2679,7 +2691,7 @@
         <v>23</v>
       </c>
       <c r="B30" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C30" s="25" t="s">
@@ -2719,7 +2731,7 @@
         <v>24</v>
       </c>
       <c r="B31" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C31" s="25" t="s">
@@ -2759,7 +2771,7 @@
         <v>25</v>
       </c>
       <c r="B32" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C32" s="25" t="s">
@@ -2796,7 +2808,7 @@
         <v>26</v>
       </c>
       <c r="B33" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C33" s="30" t="s">
@@ -2836,7 +2848,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C34" s="17" t="s">
@@ -2876,7 +2888,7 @@
         <v>29</v>
       </c>
       <c r="B35" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C35" s="15" t="s">
@@ -2912,7 +2924,7 @@
         <v>30</v>
       </c>
       <c r="B36" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C36" s="17" t="s">
@@ -2948,7 +2960,7 @@
         <v>31</v>
       </c>
       <c r="B37" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C37" s="17" t="s">
@@ -2986,7 +2998,7 @@
         <v>32</v>
       </c>
       <c r="B38" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C38" s="17" t="s">
@@ -3026,7 +3038,7 @@
         <v>33</v>
       </c>
       <c r="B39" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C39" s="17" t="s">
@@ -3064,7 +3076,7 @@
         <v>34</v>
       </c>
       <c r="B40" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C40" s="17" t="s">
@@ -3104,7 +3116,7 @@
         <v>35</v>
       </c>
       <c r="B41" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C41" s="27" t="s">
@@ -3145,7 +3157,7 @@
         <v>36</v>
       </c>
       <c r="B42" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C42" s="27" t="s">
@@ -3183,7 +3195,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C43" s="17" t="s">
@@ -3209,7 +3221,7 @@
         <v>38</v>
       </c>
       <c r="B44" s="15">
-        <f>(4*G97)</f>
+        <f>(4*G98)</f>
         <v>4</v>
       </c>
       <c r="C44" s="27" t="s">
@@ -3249,7 +3261,7 @@
         <v>39</v>
       </c>
       <c r="B45" s="15">
-        <f>(7*G97)</f>
+        <f>(7*G98)</f>
         <v>7</v>
       </c>
       <c r="C45" s="27" t="s">
@@ -3289,7 +3301,7 @@
         <v>40</v>
       </c>
       <c r="B46" s="15">
-        <f>(4*G97)</f>
+        <f>(4*G98)</f>
         <v>4</v>
       </c>
       <c r="C46" s="17" t="s">
@@ -3334,7 +3346,7 @@
         <v>41</v>
       </c>
       <c r="B47" s="15">
-        <f>(18*G97)</f>
+        <f>(18*G98)</f>
         <v>18</v>
       </c>
       <c r="C47" s="17" t="s">
@@ -3372,34 +3384,32 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A48" s="34">
-        <v>42</v>
-      </c>
+      <c r="A48" s="33"/>
       <c r="B48" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C48" s="27" t="s">
-        <v>50</v>
+      <c r="C48" s="17" t="s">
+        <v>383</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>206</v>
+        <v>214</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>204</v>
+        <v>385</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>386</v>
       </c>
       <c r="G48" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H48" s="19">
         <f t="shared" si="2"/>
-        <v>0.2</v>
+        <v>0.16</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>51</v>
+        <v>384</v>
       </c>
       <c r="J48" s="20" t="s">
         <v>167</v>
@@ -3407,38 +3417,42 @@
       <c r="K48" s="17" t="s">
         <v>169</v>
       </c>
+      <c r="L48" t="s">
+        <v>216</v>
+      </c>
       <c r="M48" s="1"/>
       <c r="N48" s="1"/>
+      <c r="R48" s="2"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A49" s="33">
-        <v>43</v>
+      <c r="A49" s="34">
+        <v>42</v>
       </c>
       <c r="B49" s="15">
-        <f>(3*G97)</f>
-        <v>3</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C49" s="27" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E49" s="15" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G49" s="19">
         <v>0.1</v>
       </c>
       <c r="H49" s="19">
         <f t="shared" si="2"/>
-        <v>0.30000000000000004</v>
+        <v>0.2</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>210</v>
+        <v>51</v>
       </c>
       <c r="J49" s="20" t="s">
         <v>167</v>
@@ -3446,41 +3460,38 @@
       <c r="K49" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L49" t="s">
-        <v>211</v>
-      </c>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A50" s="33">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>54</v>
+        <f>(3*G98)</f>
+        <v>3</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>53</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="E50" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="F50" s="15" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G50" s="19">
-        <v>0.08</v>
+        <v>0.1</v>
       </c>
       <c r="H50" s="19">
         <f t="shared" si="2"/>
-        <v>0.08</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="J50" s="20" t="s">
         <v>167</v>
@@ -3489,40 +3500,40 @@
         <v>169</v>
       </c>
       <c r="L50" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A51" s="34">
-        <v>45</v>
+      <c r="A51" s="33">
+        <v>44</v>
       </c>
       <c r="B51" s="15">
-        <f>(5*G97)</f>
-        <v>5</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="E51" s="15" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G51" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H51" s="19">
-        <f t="shared" ref="H51:H88" si="3">(B51*G51)</f>
-        <v>0.5</v>
+        <f t="shared" si="2"/>
+        <v>0.08</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J51" s="20" t="s">
         <v>167</v>
@@ -3530,202 +3541,204 @@
       <c r="K51" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L51" s="3" t="s">
+      <c r="L51" t="s">
+        <v>216</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="34">
+        <v>45</v>
+      </c>
+      <c r="B52" s="15">
+        <f>(5*G98)</f>
+        <v>5</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="G52" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H52" s="19">
+        <f t="shared" ref="H52:H89" si="3">(B52*G52)</f>
+        <v>0.5</v>
+      </c>
+      <c r="I52" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J52" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K52" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L52" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="R51" s="2" t="s">
+      <c r="R52" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A52" s="33">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="33">
         <v>46</v>
       </c>
-      <c r="B52" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C52" s="17" t="s">
+      <c r="B53" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C53" s="17" t="s">
         <v>376</v>
       </c>
-      <c r="D52" s="17" t="s">
+      <c r="D53" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E53" s="17" t="s">
         <v>220</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F53" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="G52" s="19">
+      <c r="G53" s="19">
         <v>0.08</v>
       </c>
-      <c r="H52" s="19">
+      <c r="H53" s="19">
         <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I53" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="J52" s="20" t="s">
+      <c r="J53" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="K52" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L52" s="3" t="s">
+      <c r="K53" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L53" s="3" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A53" s="33">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="33">
         <v>47</v>
       </c>
-      <c r="B53" s="15">
-        <f>(2*G97)</f>
+      <c r="B54" s="15">
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E54" s="17" t="s">
         <v>222</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F54" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="G53" s="19">
+      <c r="G54" s="19">
         <v>0.1</v>
       </c>
-      <c r="H53" s="19">
+      <c r="H54" s="19">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I53" s="17" t="s">
+      <c r="I54" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="J53" s="20" t="s">
+      <c r="J54" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="K53" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L53" s="31" t="s">
+      <c r="K54" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L54" s="31" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A54" s="34">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="34">
         <v>48</v>
       </c>
-      <c r="B54" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C54" s="17" t="s">
+      <c r="B55" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D55" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="E54" s="15" t="s">
+      <c r="E55" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F55" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="G54" s="19">
+      <c r="G55" s="19">
         <v>0.1</v>
       </c>
-      <c r="H54" s="19">
+      <c r="H55" s="19">
         <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I55" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J54" s="20" t="s">
+      <c r="J55" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="K54" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L54" s="3" t="s">
+      <c r="K55" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L55" s="3" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="33">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A56" s="33">
         <v>49</v>
       </c>
-      <c r="B55" s="15">
-        <f>(2*G97)</f>
+      <c r="B56" s="15">
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="C56" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D56" s="17" t="s">
         <v>199</v>
       </c>
-      <c r="E55" s="15" t="s">
+      <c r="E56" s="15" t="s">
         <v>228</v>
       </c>
-      <c r="F55" s="15" t="s">
+      <c r="F56" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="G55" s="19">
+      <c r="G56" s="19">
         <v>0.1</v>
       </c>
-      <c r="H55" s="19">
+      <c r="H56" s="19">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I56" s="17" t="s">
         <v>64</v>
-      </c>
-      <c r="J55" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="K55" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A56" s="33">
-        <v>50</v>
-      </c>
-      <c r="B56" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C56" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>231</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>229</v>
-      </c>
-      <c r="F56" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="G56" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="H56" s="19">
-        <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I56" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="J56" s="20" t="s">
         <v>167</v>
@@ -3733,29 +3746,29 @@
       <c r="K56" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L56" t="s">
-        <v>232</v>
+      <c r="L56" s="3" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A57" s="34">
-        <v>51</v>
+      <c r="A57" s="33">
+        <v>50</v>
       </c>
       <c r="B57" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="E57" s="15" t="s">
-        <v>233</v>
-      </c>
-      <c r="F57" s="15" t="s">
-        <v>234</v>
+        <v>65</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>230</v>
       </c>
       <c r="G57" s="19">
         <v>0.1</v>
@@ -3765,7 +3778,7 @@
         <v>0.1</v>
       </c>
       <c r="I57" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J57" s="20" t="s">
         <v>167</v>
@@ -3773,39 +3786,39 @@
       <c r="K57" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L57" s="3" t="s">
-        <v>201</v>
+      <c r="L57" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A58" s="33">
-        <v>52</v>
+      <c r="A58" s="34">
+        <v>51</v>
       </c>
       <c r="B58" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C58" s="17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G58" s="19">
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="H58" s="19">
         <f t="shared" si="3"/>
-        <v>0.09</v>
+        <v>0.1</v>
       </c>
       <c r="I58" s="17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J58" s="20" t="s">
         <v>167</v>
@@ -3814,38 +3827,38 @@
         <v>169</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A59" s="33">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B59" s="15">
-        <f>(8*G97)</f>
-        <v>8</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C59" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D59" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="E59" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="F59" s="21" t="s">
-        <v>243</v>
+        <v>69</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="F59" s="15" t="s">
+        <v>237</v>
       </c>
       <c r="G59" s="19">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="H59" s="19">
         <f t="shared" si="3"/>
-        <v>0.64</v>
+        <v>0.09</v>
       </c>
       <c r="I59" s="17" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="J59" s="20" t="s">
         <v>167</v>
@@ -3853,37 +3866,39 @@
       <c r="K59" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L59" s="3"/>
+      <c r="L59" s="3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A60" s="34">
-        <v>54</v>
+      <c r="A60" s="33">
+        <v>53</v>
       </c>
       <c r="B60" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
+        <f>(8*G98)</f>
+        <v>8</v>
       </c>
       <c r="C60" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>250</v>
+        <v>239</v>
+      </c>
+      <c r="E60" s="21" t="s">
+        <v>242</v>
       </c>
       <c r="F60" s="21" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="G60" s="19">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="H60" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.64</v>
       </c>
       <c r="I60" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J60" s="20" t="s">
         <v>167</v>
@@ -3891,39 +3906,37 @@
       <c r="K60" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L60" s="3" t="s">
-        <v>253</v>
-      </c>
+      <c r="L60" s="3"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A61" s="33">
-        <v>55</v>
+      <c r="A61" s="34">
+        <v>54</v>
       </c>
       <c r="B61" s="15">
-        <f>(8*G97)</f>
-        <v>8</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C61" s="17" t="s">
-        <v>248</v>
+        <v>72</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>241</v>
+        <v>252</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>250</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="G61" s="19">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="H61" s="19">
         <f t="shared" si="3"/>
-        <v>0.32</v>
+        <v>0.1</v>
       </c>
       <c r="I61" s="17" t="s">
-        <v>249</v>
+        <v>74</v>
       </c>
       <c r="J61" s="20" t="s">
         <v>167</v>
@@ -3931,117 +3944,117 @@
       <c r="K61" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L61" s="3"/>
+      <c r="L61" s="3" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A62" s="33">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B62" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C62" s="32" t="s">
-        <v>244</v>
+        <f>(8*G98)</f>
+        <v>8</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>248</v>
       </c>
       <c r="D62" s="20" t="s">
         <v>239</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="F62" s="21" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="G62" s="19">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="H62" s="19">
         <f t="shared" si="3"/>
-        <v>0.02</v>
+        <v>0.32</v>
       </c>
       <c r="I62" s="17" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="J62" s="20" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="K62" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L62" s="3" t="s">
-        <v>247</v>
-      </c>
+      <c r="L62" s="3"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A63" s="34">
-        <v>57</v>
+      <c r="A63" s="33">
+        <v>56</v>
       </c>
       <c r="B63" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C63" s="17" t="s">
-        <v>76</v>
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>244</v>
       </c>
       <c r="D63" s="20" t="s">
         <v>239</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F63" s="21" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="G63" s="19">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="H63" s="19">
         <f t="shared" si="3"/>
+        <v>0.02</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="J63" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="K63" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A64" s="34">
+        <v>57</v>
+      </c>
+      <c r="B64" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>239</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="G64" s="19">
         <v>0.04</v>
-      </c>
-      <c r="I63" s="17" t="s">
-        <v>254</v>
-      </c>
-      <c r="J63" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="K63" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L63" s="3" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A64" s="33">
-        <v>58</v>
-      </c>
-      <c r="B64" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C64" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D64" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="E64" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="F64" s="21" t="s">
-        <v>259</v>
-      </c>
-      <c r="G64" s="19">
-        <v>0.11</v>
       </c>
       <c r="H64" s="19">
         <f t="shared" si="3"/>
-        <v>0.11</v>
+        <v>0.04</v>
       </c>
       <c r="I64" s="17" t="s">
-        <v>80</v>
+        <v>254</v>
       </c>
       <c r="J64" s="20" t="s">
         <v>167</v>
@@ -4049,37 +4062,39 @@
       <c r="K64" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L64" s="3"/>
+      <c r="L64" s="3" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A65" s="33">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" s="15">
-        <f>(2*G97)</f>
-        <v>2</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C65" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>369</v>
+        <v>258</v>
       </c>
       <c r="F65" s="21" t="s">
-        <v>370</v>
+        <v>259</v>
       </c>
       <c r="G65" s="19">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
       <c r="H65" s="19">
         <f t="shared" si="3"/>
-        <v>0.4</v>
+        <v>0.11</v>
       </c>
       <c r="I65" s="17" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J65" s="20" t="s">
         <v>167</v>
@@ -4087,67 +4102,67 @@
       <c r="K65" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L65" s="3" t="s">
-        <v>260</v>
-      </c>
+      <c r="L65" s="3"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A66" s="34">
-        <v>60</v>
+      <c r="A66" s="33">
+        <v>59</v>
       </c>
       <c r="B66" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C66" s="17" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>262</v>
+        <v>369</v>
       </c>
       <c r="F66" s="21" t="s">
-        <v>263</v>
+        <v>370</v>
       </c>
       <c r="G66" s="19">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H66" s="19">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="I66" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J66" s="20" t="s">
-        <v>194</v>
+        <v>167</v>
       </c>
       <c r="K66" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L66" s="3"/>
+      <c r="L66" s="3" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A67" s="33">
-        <v>61</v>
+      <c r="A67" s="34">
+        <v>60</v>
       </c>
       <c r="B67" s="15">
-        <f>(2*G97)</f>
+        <f>(2*G98)</f>
         <v>2</v>
       </c>
       <c r="C67" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G67" s="19">
         <v>0.5</v>
@@ -4157,7 +4172,7 @@
         <v>1</v>
       </c>
       <c r="I67" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J67" s="20" t="s">
         <v>194</v>
@@ -4165,39 +4180,37 @@
       <c r="K67" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L67" s="3" t="s">
-        <v>260</v>
-      </c>
+      <c r="L67" s="3"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A68" s="33">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B68" s="15">
-        <f>(3*G97)</f>
-        <v>3</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C68" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G68" s="19">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="H68" s="19">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>1</v>
       </c>
       <c r="I68" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J68" s="20" t="s">
         <v>194</v>
@@ -4206,240 +4219,242 @@
         <v>169</v>
       </c>
       <c r="L68" s="3" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A69" s="34">
-        <v>63</v>
+      <c r="A69" s="33">
+        <v>62</v>
       </c>
       <c r="B69" s="15">
-        <f>(7*G97)</f>
-        <v>7</v>
-      </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="F69" s="15" t="s">
-        <v>183</v>
+        <f>(3*G98)</f>
+        <v>3</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="E69" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="F69" s="21" t="s">
+        <v>267</v>
       </c>
       <c r="G69" s="19">
-        <v>0.31</v>
+        <v>0.1</v>
       </c>
       <c r="H69" s="19">
         <f t="shared" si="3"/>
-        <v>2.17</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I69" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="J69" s="20"/>
-      <c r="K69" s="17"/>
+        <v>84</v>
+      </c>
+      <c r="J69" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="K69" s="17" t="s">
+        <v>169</v>
+      </c>
       <c r="L69" s="3" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A70" s="33">
-        <v>64</v>
+      <c r="A70" s="34">
+        <v>63</v>
       </c>
       <c r="B70" s="15">
-        <f>(14*G97)</f>
-        <v>14</v>
+        <f>(7*G98)</f>
+        <v>7</v>
       </c>
       <c r="C70" s="17"/>
       <c r="D70" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E70" s="15">
-        <v>1722533123</v>
+      <c r="E70" s="15" t="s">
+        <v>184</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="G70" s="19">
-        <v>0.152</v>
+        <v>0.31</v>
       </c>
       <c r="H70" s="19">
         <f t="shared" si="3"/>
-        <v>2.1280000000000001</v>
+        <v>2.17</v>
       </c>
       <c r="I70" s="17" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J70" s="20"/>
       <c r="K70" s="17"/>
       <c r="L70" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A71" s="33">
+        <v>64</v>
+      </c>
+      <c r="B71" s="15">
+        <f>(14*G98)</f>
+        <v>14</v>
+      </c>
+      <c r="C71" s="17"/>
+      <c r="D71" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="E71" s="15">
+        <v>1722533123</v>
+      </c>
+      <c r="F71" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="G71" s="19">
+        <v>0.152</v>
+      </c>
+      <c r="H71" s="19">
+        <f t="shared" si="3"/>
+        <v>2.1280000000000001</v>
+      </c>
+      <c r="I71" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="J71" s="20"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="R70" s="2" t="s">
+      <c r="R71" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="37"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="38"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="37"/>
-      <c r="G71" s="39"/>
-      <c r="H71" s="39"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="40"/>
-      <c r="K71" s="37"/>
-      <c r="L71" s="3"/>
-    </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A72" s="35">
-        <v>1</v>
-      </c>
-      <c r="B72" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C72" s="17" t="s">
+      <c r="A72" s="37"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="37"/>
+      <c r="G72" s="39"/>
+      <c r="H72" s="39"/>
+      <c r="I72" s="38"/>
+      <c r="J72" s="40"/>
+      <c r="K72" s="37"/>
+      <c r="L72" s="3"/>
+    </row>
+    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A73" s="35">
+        <v>1</v>
+      </c>
+      <c r="B73" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C73" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="17" t="s">
+      <c r="D73" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="E72" s="17" t="s">
+      <c r="E73" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F72" s="15" t="s">
+      <c r="F73" s="15" t="s">
         <v>134</v>
       </c>
-      <c r="G72" s="19">
+      <c r="G73" s="19">
         <v>1.4</v>
       </c>
-      <c r="H72" s="19">
+      <c r="H73" s="19">
         <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
-      <c r="I72" s="17" t="s">
+      <c r="I73" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="J72" s="20" t="s">
+      <c r="J73" s="20" t="s">
         <v>271</v>
       </c>
-      <c r="K72" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L72" s="3"/>
-    </row>
-    <row r="73" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="35">
+      <c r="K73" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L73" s="3"/>
+    </row>
+    <row r="74" spans="1:18" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="35">
         <v>2</v>
       </c>
-      <c r="B73" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C73" s="17" t="s">
+      <c r="B74" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C74" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D73" s="17" t="s">
+      <c r="D74" s="17" t="s">
         <v>357</v>
       </c>
-      <c r="E73" s="17" t="s">
+      <c r="E74" s="17" t="s">
         <v>353</v>
       </c>
-      <c r="F73" s="15" t="s">
+      <c r="F74" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="G73" s="19">
+      <c r="G74" s="19">
         <v>0.64</v>
       </c>
-      <c r="H73" s="19">
+      <c r="H74" s="19">
         <f t="shared" si="3"/>
         <v>0.64</v>
       </c>
-      <c r="I73" s="17" t="s">
+      <c r="I74" s="17" t="s">
         <v>355</v>
       </c>
-      <c r="J73" s="20" t="s">
+      <c r="J74" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="K73" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L73" s="3"/>
-    </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A74" s="35">
+      <c r="K74" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L74" s="3"/>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A75" s="35">
         <v>3</v>
       </c>
-      <c r="B74" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C74" s="17" t="s">
+      <c r="B75" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C75" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D75" s="17" t="s">
         <v>114</v>
       </c>
-      <c r="E74" s="17" t="s">
+      <c r="E75" s="17" t="s">
         <v>349</v>
       </c>
-      <c r="F74" s="15" t="s">
+      <c r="F75" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="G74" s="19">
+      <c r="G75" s="19">
         <v>1.24</v>
       </c>
-      <c r="H74" s="19">
+      <c r="H75" s="19">
         <f t="shared" si="3"/>
         <v>1.24</v>
       </c>
-      <c r="I74" s="17" t="s">
+      <c r="I75" s="17" t="s">
         <v>351</v>
       </c>
-      <c r="J74" s="20" t="s">
+      <c r="J75" s="20" t="s">
         <v>352</v>
-      </c>
-      <c r="K74" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L74" s="3"/>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A75" s="35">
-        <v>4</v>
-      </c>
-      <c r="B75" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C75" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="D75" s="25" t="s">
-        <v>122</v>
-      </c>
-      <c r="E75" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F75" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="G75" s="19">
-        <v>5.66</v>
-      </c>
-      <c r="H75" s="19">
-        <f>(B75*G75)</f>
-        <v>5.66</v>
-      </c>
-      <c r="I75" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="J75" s="20" t="s">
-        <v>345</v>
       </c>
       <c r="K75" s="17" t="s">
         <v>169</v>
@@ -4448,262 +4463,262 @@
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A76" s="35">
+        <v>4</v>
+      </c>
+      <c r="B76" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D76" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E76" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F76" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76" s="19">
+        <v>5.66</v>
+      </c>
+      <c r="H76" s="19">
+        <f>(B76*G76)</f>
+        <v>5.66</v>
+      </c>
+      <c r="I76" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="J76" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="K76" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L76" s="3"/>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A77" s="35">
         <v>5</v>
       </c>
-      <c r="B76" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C76" s="17" t="s">
+      <c r="B77" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C77" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D76" s="17" t="s">
+      <c r="D77" s="17" t="s">
         <v>311</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E77" s="17" t="s">
         <v>371</v>
       </c>
-      <c r="F76" s="15" t="s">
+      <c r="F77" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="G76" s="19">
+      <c r="G77" s="19">
         <v>2.84</v>
       </c>
-      <c r="H76" s="19">
+      <c r="H77" s="19">
         <f t="shared" si="3"/>
         <v>2.84</v>
       </c>
-      <c r="I76" s="17" t="s">
+      <c r="I77" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="J76" s="20" t="s">
+      <c r="J77" s="20" t="s">
         <v>273</v>
       </c>
-      <c r="K76" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L76" s="3"/>
-      <c r="R76" s="2" t="s">
+      <c r="K77" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L77" s="3"/>
+      <c r="R77" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A77" s="35">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A78" s="35">
         <v>6</v>
       </c>
-      <c r="B77" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C77" s="17" t="s">
+      <c r="B78" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C78" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D78" s="17" t="s">
         <v>312</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E78" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="F77" s="15" t="s">
+      <c r="F78" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G77" s="19">
+      <c r="G78" s="19">
         <v>0.86</v>
       </c>
-      <c r="H77" s="19">
+      <c r="H78" s="19">
         <f t="shared" si="3"/>
         <v>0.86</v>
       </c>
-      <c r="I77" s="17" t="s">
+      <c r="I78" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="J77" s="20" t="s">
+      <c r="J78" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="K77" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L77" s="3"/>
-    </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A78" s="35">
+      <c r="K78" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L78" s="3"/>
+    </row>
+    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A79" s="35">
         <v>7</v>
       </c>
-      <c r="B78" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C78" s="17" t="s">
+      <c r="B79" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C79" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D78" s="17" t="s">
+      <c r="D79" s="17" t="s">
         <v>297</v>
       </c>
-      <c r="E78" s="15" t="s">
+      <c r="E79" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="F78" s="15" t="s">
+      <c r="F79" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="G78" s="19">
+      <c r="G79" s="19">
         <v>0.15</v>
       </c>
-      <c r="H78" s="19">
+      <c r="H79" s="19">
         <f t="shared" si="3"/>
         <v>0.15</v>
       </c>
-      <c r="I78" s="17" t="s">
+      <c r="I79" s="17" t="s">
         <v>217</v>
       </c>
-      <c r="J78" s="20" t="s">
+      <c r="J79" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="K78" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L78" s="3"/>
-    </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A79" s="35">
+      <c r="K79" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L79" s="3"/>
+    </row>
+    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A80" s="35">
         <v>8</v>
       </c>
-      <c r="B79" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C79" s="17" t="s">
+      <c r="B80" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C80" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D79" s="17" t="s">
+      <c r="D80" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E79" s="17" t="s">
+      <c r="E80" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="F79" s="15" t="s">
+      <c r="F80" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="G79" s="19">
+      <c r="G80" s="19">
         <v>0.67</v>
       </c>
-      <c r="H79" s="19">
+      <c r="H80" s="19">
         <f t="shared" si="3"/>
         <v>0.67</v>
       </c>
-      <c r="I79" s="17" t="s">
+      <c r="I80" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="J79" s="20" t="s">
+      <c r="J80" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="K79" s="17" t="s">
+      <c r="K80" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="L79" s="3"/>
-    </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A80" s="35">
-        <v>9</v>
-      </c>
-      <c r="B80" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C80" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D80" s="17"/>
-      <c r="E80" s="15"/>
-      <c r="F80" s="15"/>
-      <c r="G80" s="19"/>
-      <c r="H80" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I80" s="17"/>
-      <c r="J80" s="20"/>
-      <c r="K80" s="15"/>
       <c r="L80" s="3"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="35">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B81" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C81" s="17" t="s">
-        <v>89</v>
+        <v>45</v>
       </c>
       <c r="D81" s="17"/>
+      <c r="E81" s="15"/>
       <c r="F81" s="15"/>
       <c r="G81" s="19"/>
       <c r="H81" s="19">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
+      <c r="I81" s="17"/>
       <c r="J81" s="20"/>
       <c r="K81" s="15"/>
       <c r="L81" s="3"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="35">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B82" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="D82" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="E82" s="15" t="s">
-        <v>287</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>288</v>
-      </c>
-      <c r="G82" s="19">
-        <v>0.1</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D82" s="17"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="19"/>
       <c r="H82" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
-      </c>
-      <c r="I82" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="J82" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="K82" s="17" t="s">
-        <v>169</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J82" s="20"/>
+      <c r="K82" s="15"/>
       <c r="L82" s="3"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="35">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B83" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E83" s="15" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="F83" s="15" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="G83" s="19">
         <v>0.1</v>
@@ -4713,7 +4728,7 @@
         <v>0.1</v>
       </c>
       <c r="I83" s="17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J83" s="20" t="s">
         <v>195</v>
@@ -4725,33 +4740,33 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="35">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B84" s="15">
-        <f>(3*G97)</f>
-        <v>3</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>347</v>
+        <v>100</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="E84" s="15" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="F84" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G84" s="19">
         <v>0.1</v>
       </c>
       <c r="H84" s="19">
         <f t="shared" si="3"/>
-        <v>0.30000000000000004</v>
+        <v>0.1</v>
       </c>
       <c r="I84" s="17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J84" s="20" t="s">
         <v>195</v>
@@ -4759,39 +4774,37 @@
       <c r="K84" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L84" s="3" t="s">
-        <v>216</v>
-      </c>
+      <c r="L84" s="3"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="35">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B85" s="15">
-        <f>(2*G97)</f>
-        <v>2</v>
+        <f>(3*G98)</f>
+        <v>3</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>103</v>
+        <v>347</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="E85" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F85" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="G85" s="19">
         <v>0.1</v>
       </c>
       <c r="H85" s="19">
         <f t="shared" si="3"/>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="I85" s="17" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="J85" s="20" t="s">
         <v>195</v>
@@ -4800,38 +4813,38 @@
         <v>169</v>
       </c>
       <c r="L85" s="3" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="35">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B86" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
+        <f>(2*G98)</f>
+        <v>2</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="E86" s="15" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F86" s="15" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="G86" s="19">
         <v>0.1</v>
       </c>
       <c r="H86" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I86" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J86" s="20" t="s">
         <v>195</v>
@@ -4840,116 +4853,116 @@
         <v>169</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>291</v>
+        <v>201</v>
       </c>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="35">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B87" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="E87" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="F87" s="21" t="s">
-        <v>358</v>
+        <v>214</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>289</v>
+      </c>
+      <c r="F87" s="15" t="s">
+        <v>290</v>
       </c>
       <c r="G87" s="19">
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="H87" s="19">
         <f t="shared" si="3"/>
-        <v>0.37</v>
+        <v>0.1</v>
       </c>
       <c r="I87" s="17" t="s">
-        <v>348</v>
+        <v>58</v>
       </c>
       <c r="J87" s="20" t="s">
-        <v>280</v>
+        <v>195</v>
       </c>
       <c r="K87" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L87" s="3"/>
+      <c r="L87" s="3" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="35">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B88" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C88" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>214</v>
+        <v>360</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="G88" s="19">
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="H88" s="19">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.37</v>
       </c>
       <c r="I88" s="17" t="s">
-        <v>49</v>
+        <v>348</v>
       </c>
       <c r="J88" s="20" t="s">
-        <v>195</v>
+        <v>280</v>
       </c>
       <c r="K88" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L88" s="3" t="s">
-        <v>291</v>
-      </c>
+      <c r="L88" s="3"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A89" s="35">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B89" s="15">
-        <f>(5*G97)</f>
-        <v>5</v>
+        <f>(1*G98)</f>
+        <v>1</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>367</v>
+        <v>106</v>
       </c>
       <c r="D89" s="17" t="s">
-        <v>239</v>
-      </c>
-      <c r="E89" s="20" t="s">
-        <v>292</v>
+        <v>214</v>
+      </c>
+      <c r="E89" s="21" t="s">
+        <v>361</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>293</v>
+        <v>362</v>
       </c>
       <c r="G89" s="19">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="H89" s="19">
-        <f>(B89*G89)</f>
-        <v>0.25</v>
+        <f t="shared" si="3"/>
+        <v>0.1</v>
       </c>
       <c r="I89" s="17" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="J89" s="20" t="s">
         <v>195</v>
@@ -4957,203 +4970,243 @@
       <c r="K89" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L89" s="2" t="s">
-        <v>294</v>
+      <c r="L89" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A90" s="35">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B90" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
+        <f>(5*G98)</f>
+        <v>5</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>279</v>
-      </c>
-      <c r="D90" s="20" t="s">
-        <v>252</v>
+        <v>367</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>239</v>
       </c>
       <c r="E90" s="20" t="s">
-        <v>250</v>
+        <v>292</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>251</v>
+        <v>293</v>
       </c>
       <c r="G90" s="19">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H90" s="19">
-        <f t="shared" ref="H90:H93" si="4">(B90*G90)</f>
-        <v>0.1</v>
+        <f>(B90*G90)</f>
+        <v>0.25</v>
       </c>
       <c r="I90" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J90" s="20" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="K90" s="17" t="s">
         <v>169</v>
       </c>
-      <c r="L90" s="2"/>
+      <c r="L90" s="2" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A91" s="35">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B91" s="15">
-        <f>(1*G97)</f>
+        <f>(1*G98)</f>
         <v>1</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D91" s="20" t="s">
         <v>252</v>
       </c>
-      <c r="E91" s="21" t="s">
+      <c r="E91" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="F91" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="G91" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="H91" s="19">
+        <f t="shared" ref="H91:H94" si="4">(B91*G91)</f>
+        <v>0.1</v>
+      </c>
+      <c r="I91" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="J91" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="K91" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A92" s="35">
+        <v>22</v>
+      </c>
+      <c r="B92" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="E92" s="21" t="s">
         <v>258</v>
       </c>
-      <c r="F91" s="21" t="s">
+      <c r="F92" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="G91" s="19">
+      <c r="G92" s="19">
         <v>0.11</v>
       </c>
-      <c r="H91" s="19">
+      <c r="H92" s="19">
         <f t="shared" si="4"/>
         <v>0.11</v>
       </c>
-      <c r="I91" s="17" t="s">
+      <c r="I92" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="J91" s="20" t="s">
+      <c r="J92" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="K91" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="L91" s="2"/>
-    </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A92" s="35">
+      <c r="K92" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="L92" s="2"/>
+    </row>
+    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A93" s="35">
         <v>23</v>
       </c>
-      <c r="B92" s="15">
-        <f>(6*G97)</f>
+      <c r="B93" s="15">
+        <f>(6*G98)</f>
         <v>6</v>
       </c>
-      <c r="C92" s="17"/>
-      <c r="D92" s="17" t="s">
+      <c r="C93" s="17"/>
+      <c r="D93" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E93" s="15">
         <v>500588000</v>
       </c>
-      <c r="F92" s="15" t="s">
+      <c r="F93" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="G92" s="19">
+      <c r="G93" s="19">
         <v>0.1</v>
       </c>
-      <c r="H92" s="19">
+      <c r="H93" s="19">
         <f t="shared" si="4"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="I92" s="27" t="s">
+      <c r="I93" s="27" t="s">
         <v>363</v>
       </c>
-      <c r="J92" s="20"/>
-      <c r="K92" s="17"/>
-      <c r="R92" s="2" t="s">
+      <c r="J93" s="20"/>
+      <c r="K93" s="17"/>
+      <c r="R93" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A93" s="35">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A94" s="35">
         <v>24</v>
       </c>
-      <c r="B93" s="15">
-        <f>(1*G97)</f>
-        <v>1</v>
-      </c>
-      <c r="C93" s="15"/>
-      <c r="D93" s="17" t="s">
+      <c r="B94" s="15">
+        <f>(1*G98)</f>
+        <v>1</v>
+      </c>
+      <c r="C94" s="15"/>
+      <c r="D94" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E93" s="15" t="s">
+      <c r="E94" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="F93" s="15" t="s">
+      <c r="F94" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="G93" s="19">
+      <c r="G94" s="19">
         <v>0.36</v>
       </c>
-      <c r="H93" s="19">
+      <c r="H94" s="19">
         <f t="shared" si="4"/>
         <v>0.36</v>
       </c>
-      <c r="I93" s="27"/>
-      <c r="J93" s="15"/>
-      <c r="K93" s="15"/>
-    </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A94" s="1"/>
-    </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="I96" s="12"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="15"/>
+    </row>
+    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A95" s="1"/>
     </row>
     <row r="97" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="F97" s="44" t="s">
+      <c r="I97" s="12"/>
+    </row>
+    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F98" s="44" t="s">
         <v>368</v>
       </c>
-      <c r="G97" s="1">
-        <v>1</v>
-      </c>
-      <c r="H97" s="10" t="s">
+      <c r="G98" s="1">
+        <v>1</v>
+      </c>
+      <c r="H98" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="I97" s="5"/>
-    </row>
-    <row r="98" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H98" s="9">
-        <f>SUM(H12:H70)</f>
-        <v>75.257999999999996</v>
-      </c>
       <c r="I98" s="5"/>
     </row>
     <row r="99" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H99" s="1"/>
-      <c r="I99" s="6"/>
+      <c r="H99" s="9">
+        <f>SUM(H12:H71)</f>
+        <v>75.417999999999992</v>
+      </c>
+      <c r="I99" s="5"/>
     </row>
     <row r="100" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H100" s="7" t="s">
+      <c r="H100" s="1"/>
+      <c r="I100" s="6"/>
+    </row>
+    <row r="101" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H101" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="I100" s="3"/>
-    </row>
-    <row r="101" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H101" s="9">
-        <f>SUM(H72:H93)</f>
+      <c r="I101" s="3"/>
+    </row>
+    <row r="102" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H102" s="9">
+        <f>SUM(H73:H94)</f>
         <v>16.149999999999999</v>
       </c>
     </row>
-    <row r="103" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H103" s="7" t="s">
+    <row r="104" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H104" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H104" s="9">
-        <f>SUM(H98+H101)</f>
-        <v>91.407999999999987</v>
-      </c>
-    </row>
-    <row r="110" spans="6:9" x14ac:dyDescent="0.2">
-      <c r="H110" s="11"/>
+    <row r="105" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H105" s="9">
+        <f>SUM(H99+H102)</f>
+        <v>91.567999999999984</v>
+      </c>
+    </row>
+    <row r="111" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="H111" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>